<commit_message>
Added Pere Marquette rolling stock
</commit_message>
<xml_diff>
--- a/trains/Inventory.xlsx
+++ b/trains/Inventory.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="171">
   <si>
     <t>Road Name</t>
   </si>
@@ -436,6 +436,108 @@
   </si>
   <si>
     <t>Evans double plug door</t>
+  </si>
+  <si>
+    <t>bobber caboose</t>
+  </si>
+  <si>
+    <t>40' quad hopper</t>
+  </si>
+  <si>
+    <t>70 ton 2 bay covered hopper</t>
+  </si>
+  <si>
+    <t>Bowser</t>
+  </si>
+  <si>
+    <t>40' 1937 AAR boxcar</t>
+  </si>
+  <si>
+    <t>45761-08</t>
+  </si>
+  <si>
+    <t>less 30% sale?</t>
+  </si>
+  <si>
+    <t>45761-07</t>
+  </si>
+  <si>
+    <t>eBay?</t>
+  </si>
+  <si>
+    <t>Evans gondola</t>
+  </si>
+  <si>
+    <t>train show at temple</t>
+  </si>
+  <si>
+    <t>Alco RS3</t>
+  </si>
+  <si>
+    <t>maroon+gold</t>
+  </si>
+  <si>
+    <t>eBay - brianweismanjbw</t>
+  </si>
+  <si>
+    <t>$3.34 shipping</t>
+  </si>
+  <si>
+    <t>52'6" drop end mill gondola</t>
+  </si>
+  <si>
+    <t>45765-05</t>
+  </si>
+  <si>
+    <t>45765-06</t>
+  </si>
+  <si>
+    <t>45765-03</t>
+  </si>
+  <si>
+    <t>45765-04</t>
+  </si>
+  <si>
+    <t>flatcar</t>
+  </si>
+  <si>
+    <t>48715-01?</t>
+  </si>
+  <si>
+    <t>train show - Springfield</t>
+  </si>
+  <si>
+    <t>A913</t>
+  </si>
+  <si>
+    <t>eBay</t>
+  </si>
+  <si>
+    <t>A471</t>
+  </si>
+  <si>
+    <t>DM&amp;IR class G2 wood caboose</t>
+  </si>
+  <si>
+    <t>920-103455</t>
+  </si>
+  <si>
+    <t>$3.07 shipping</t>
+  </si>
+  <si>
+    <t>PM 18878</t>
+  </si>
+  <si>
+    <t>PM 18881</t>
+  </si>
+  <si>
+    <t>PM 18914</t>
+  </si>
+  <si>
+    <t>PM 18942</t>
+  </si>
+  <si>
+    <t>70 ton flat car</t>
   </si>
 </sst>
 </file>
@@ -845,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+      <selection activeCell="J6" sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,101 +1020,127 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>281</v>
+        <v>1536</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E3">
-        <v>9388</v>
+        <v>63903</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="5">
-        <v>42479</v>
+        <v>149</v>
       </c>
       <c r="H3" s="4">
-        <v>109</v>
+        <v>114.95</v>
       </c>
       <c r="I3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J3" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B4">
-        <v>405</v>
+        <v>281</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E4">
-        <v>66304</v>
+        <v>9388</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>121</v>
+      </c>
+      <c r="G4" s="5">
+        <v>42479</v>
       </c>
       <c r="H4" s="4">
-        <v>114.99</v>
+        <v>109</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B5">
-        <v>8087</v>
+        <v>405</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5">
-        <v>63211</v>
+        <v>66304</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2">
-        <v>42429</v>
+        <v>72</v>
       </c>
       <c r="H5" s="4">
-        <v>99.99</v>
+        <v>114.99</v>
       </c>
       <c r="I5" t="s">
         <v>26</v>
       </c>
       <c r="J5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>8087</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>63211</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2">
+        <v>42429</v>
+      </c>
+      <c r="H6" s="4">
+        <v>99.99</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J5">
-    <sortCondition ref="A2:A5"/>
-    <sortCondition ref="B2:B5"/>
+  <sortState ref="A2:J6">
+    <sortCondition ref="A2:A6"/>
+    <sortCondition ref="B2:B6"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1020,11 +1148,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="A1:K38"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1401,22 +1529,25 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>5544</v>
+        <v>5517</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="F14">
+        <v>40931</v>
       </c>
       <c r="G14" t="s">
         <v>88</v>
       </c>
       <c r="I14" s="4">
-        <v>12</v>
+        <v>18.95</v>
       </c>
       <c r="J14" t="s">
         <v>45</v>
@@ -1427,31 +1558,25 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>71729</v>
+        <v>5544</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D15" t="s">
         <v>29</v>
       </c>
       <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="4">
         <v>12</v>
       </c>
-      <c r="G15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="2">
-        <v>42305</v>
-      </c>
-      <c r="I15" s="4">
-        <v>4.8</v>
-      </c>
       <c r="J15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K15" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1459,31 +1584,28 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>71741</v>
+        <v>8900</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D16" t="s">
         <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>17644</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="2">
-        <v>42305</v>
+        <v>48</v>
       </c>
       <c r="I16" s="4">
-        <v>4.8</v>
+        <v>12.95</v>
       </c>
       <c r="J16" t="s">
-        <v>132</v>
-      </c>
-      <c r="K16" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1491,139 +1613,138 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>76032</v>
+        <v>9061</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>65</v>
+      </c>
+      <c r="F17">
+        <v>913</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="2">
-        <v>42305</v>
+        <v>72</v>
       </c>
       <c r="I17" s="4">
-        <v>4.8</v>
+        <v>10</v>
       </c>
       <c r="J17" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="K17" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>606902</v>
+        <v>9072</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="F18">
-        <v>19131</v>
+        <v>913</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="2">
-        <v>42680</v>
+        <v>72</v>
       </c>
       <c r="I18" s="4">
         <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K18" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>2217</v>
+        <v>71729</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
       </c>
-      <c r="F19">
-        <v>92893</v>
-      </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="H19" s="2">
-        <v>42126</v>
+        <v>42305</v>
       </c>
       <c r="I19" s="4">
-        <v>15.98</v>
+        <v>4.8</v>
       </c>
       <c r="J19" t="s">
-        <v>14</v>
+        <v>132</v>
+      </c>
+      <c r="K19" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B20">
-        <v>3202</v>
+        <v>71741</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="H20" s="2">
+        <v>42305</v>
+      </c>
       <c r="I20" s="4">
-        <v>25.95</v>
+        <v>4.8</v>
       </c>
       <c r="J20" t="s">
-        <v>69</v>
+        <v>132</v>
+      </c>
+      <c r="K20" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>3226</v>
+        <v>73035</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1632,199 +1753,194 @@
         <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="G21" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="2">
-        <v>42674</v>
-      </c>
       <c r="I21" s="4">
-        <v>17</v>
+        <v>25.95</v>
       </c>
       <c r="J21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K21" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>5006</v>
+        <v>73060</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="I22" s="4">
-        <v>15</v>
+        <v>29.95</v>
       </c>
       <c r="J22" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="K22" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>6128</v>
+        <v>76032</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
       </c>
-      <c r="F23">
-        <v>97340</v>
-      </c>
       <c r="G23" t="s">
-        <v>88</v>
+        <v>30</v>
+      </c>
+      <c r="H23" s="2">
+        <v>42305</v>
       </c>
       <c r="I23" s="4">
-        <v>31.95</v>
+        <v>4.8</v>
       </c>
       <c r="J23" t="s">
-        <v>69</v>
+        <v>132</v>
+      </c>
+      <c r="K23" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24">
-        <v>1165</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" t="s">
-        <v>78</v>
+        <v>24</v>
+      </c>
+      <c r="F24">
+        <v>18448</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="B25">
-        <v>9602</v>
+        <v>606902</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F25">
-        <v>91487</v>
+        <v>19131</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H25" s="2">
-        <v>42309</v>
+        <v>42680</v>
       </c>
       <c r="I25" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="K25" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B26">
-        <v>9621</v>
+        <v>2217</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" t="s">
-        <v>86</v>
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>92893</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H26" s="2">
-        <v>42303</v>
+        <v>42126</v>
       </c>
       <c r="I26" s="4">
-        <v>29.95</v>
+        <v>15.98</v>
       </c>
       <c r="J26" t="s">
-        <v>93</v>
-      </c>
-      <c r="K26" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B27">
-        <v>10112</v>
+        <v>3202</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27">
-        <v>89082</v>
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>115</v>
       </c>
       <c r="G27" t="s">
-        <v>83</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H27" s="2"/>
       <c r="I27" s="4">
-        <v>27.98</v>
+        <v>25.95</v>
       </c>
       <c r="J27" t="s">
         <v>69</v>
@@ -1832,336 +1948,321 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B28">
-        <v>10312</v>
+        <v>3226</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28">
-        <v>17532</v>
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
+        <v>54</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H28" s="2">
-        <v>42537</v>
+        <v>42674</v>
       </c>
       <c r="I28" s="4">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J28" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="K28" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B29">
-        <v>25907</v>
+        <v>5006</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F29" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>48</v>
+      </c>
+      <c r="I29" s="4">
+        <v>15</v>
+      </c>
+      <c r="J29" t="s">
+        <v>118</v>
+      </c>
+      <c r="K29" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B30">
-        <v>32246</v>
+        <v>6128</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F30">
-        <v>18132</v>
+        <v>97340</v>
       </c>
       <c r="G30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="2">
-        <v>42411</v>
+        <v>88</v>
       </c>
       <c r="I30" s="4">
-        <v>12.5</v>
+        <v>31.95</v>
       </c>
       <c r="J30" t="s">
-        <v>91</v>
-      </c>
-      <c r="K30" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B31">
-        <v>113894</v>
+        <v>1165</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31">
-        <v>93725</v>
+        <v>77</v>
+      </c>
+      <c r="F31" t="s">
+        <v>78</v>
       </c>
       <c r="G31" t="s">
-        <v>30</v>
-      </c>
-      <c r="H31" s="2">
-        <v>42709</v>
-      </c>
-      <c r="I31" s="4">
-        <v>10</v>
-      </c>
-      <c r="J31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B32">
-        <v>148077</v>
+        <v>9602</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
         <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>91487</v>
       </c>
       <c r="G32" t="s">
-        <v>30</v>
+        <v>48</v>
+      </c>
+      <c r="H32" s="2">
+        <v>42309</v>
       </c>
       <c r="I32" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J32" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B33">
-        <v>591263</v>
+        <v>9621</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="H33" s="2">
-        <v>42440</v>
+        <v>42303</v>
       </c>
       <c r="I33" s="4">
-        <v>14.99</v>
+        <v>29.95</v>
       </c>
       <c r="J33" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="K33" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B34">
-        <v>598016</v>
+        <v>10112</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>92957</v>
+        <v>89082</v>
       </c>
       <c r="G34" t="s">
-        <v>30</v>
-      </c>
-      <c r="H34" s="2">
-        <v>42680</v>
+        <v>83</v>
       </c>
       <c r="I34" s="4">
-        <v>14</v>
+        <v>27.98</v>
       </c>
       <c r="J34" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B35">
-        <v>675097</v>
+        <v>10312</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" t="s">
-        <v>39</v>
+        <v>24</v>
+      </c>
+      <c r="F35">
+        <v>17532</v>
       </c>
       <c r="G35" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="H35" s="2">
-        <v>42521</v>
+        <v>42537</v>
       </c>
       <c r="I35" s="4">
-        <v>16.489999999999998</v>
+        <v>11</v>
       </c>
       <c r="J35" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="K35" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B36">
-        <v>2706</v>
+        <v>25907</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36">
-        <v>92912</v>
+        <v>81</v>
+      </c>
+      <c r="F36" t="s">
+        <v>82</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="2">
-        <v>42637</v>
-      </c>
-      <c r="I36" s="4">
-        <v>13.29</v>
-      </c>
-      <c r="J36" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B37">
-        <v>14274</v>
+        <v>32246</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F37">
-        <v>5648</v>
+        <v>18132</v>
       </c>
       <c r="G37" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H37" s="2">
-        <v>42672</v>
+        <v>42411</v>
       </c>
       <c r="I37" s="4">
-        <v>7</v>
+        <v>12.5</v>
       </c>
       <c r="J37" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="K37" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B38">
-        <v>14450</v>
+        <v>113894</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>
@@ -2170,28 +2271,670 @@
         <v>12</v>
       </c>
       <c r="F38">
+        <v>93725</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="2">
+        <v>42709</v>
+      </c>
+      <c r="I38" s="4">
+        <v>10</v>
+      </c>
+      <c r="J38" t="s">
+        <v>32</v>
+      </c>
+      <c r="K38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <v>148077</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="4">
+        <v>12</v>
+      </c>
+      <c r="J39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40">
+        <v>591263</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="2">
+        <v>42440</v>
+      </c>
+      <c r="I40" s="4">
+        <v>14.99</v>
+      </c>
+      <c r="J40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41">
+        <v>598016</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41">
+        <v>92957</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="2">
+        <v>42680</v>
+      </c>
+      <c r="I41" s="4">
+        <v>14</v>
+      </c>
+      <c r="J41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42">
+        <v>675097</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="2">
+        <v>42521</v>
+      </c>
+      <c r="I42" s="4">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="J42" t="s">
+        <v>40</v>
+      </c>
+      <c r="K42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>2706</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>92912</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="2">
+        <v>42637</v>
+      </c>
+      <c r="I43" s="4">
+        <v>13.29</v>
+      </c>
+      <c r="J43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>14274</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44">
         <v>5648</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G44" t="s">
         <v>48</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H44" s="2">
         <v>42672</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I44" s="4">
         <v>7</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J44" t="s">
         <v>49</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K44" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>14450</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45">
+        <v>5648</v>
+      </c>
+      <c r="G45" t="s">
+        <v>48</v>
+      </c>
+      <c r="H45" s="2">
+        <v>42672</v>
+      </c>
+      <c r="I45" s="4">
+        <v>7</v>
+      </c>
+      <c r="J45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>16534</v>
+      </c>
+      <c r="C46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" t="s">
+        <v>158</v>
+      </c>
+      <c r="G46" t="s">
+        <v>48</v>
+      </c>
+      <c r="J46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>18878</v>
+      </c>
+      <c r="C47" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47" t="s">
+        <v>48</v>
+      </c>
+      <c r="J47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>18881</v>
+      </c>
+      <c r="C48" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" t="s">
+        <v>167</v>
+      </c>
+      <c r="G48" t="s">
+        <v>48</v>
+      </c>
+      <c r="J48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>18914</v>
+      </c>
+      <c r="C49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F49" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" t="s">
+        <v>48</v>
+      </c>
+      <c r="J49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>18942</v>
+      </c>
+      <c r="C50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" t="s">
+        <v>169</v>
+      </c>
+      <c r="G50" t="s">
+        <v>48</v>
+      </c>
+      <c r="J50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>20025</v>
+      </c>
+      <c r="C51" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" t="s">
+        <v>140</v>
+      </c>
+      <c r="F51">
+        <v>41329</v>
+      </c>
+      <c r="G51" t="s">
+        <v>48</v>
+      </c>
+      <c r="H51" s="2">
+        <v>42608</v>
+      </c>
+      <c r="I51" s="4">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="J51" t="s">
+        <v>150</v>
+      </c>
+      <c r="K51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52">
+        <v>20037</v>
+      </c>
+      <c r="C52" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" t="s">
+        <v>140</v>
+      </c>
+      <c r="F52">
+        <v>41330</v>
+      </c>
+      <c r="G52" t="s">
+        <v>48</v>
+      </c>
+      <c r="H52" s="2">
+        <v>42608</v>
+      </c>
+      <c r="I52" s="4">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="J52" t="s">
+        <v>150</v>
+      </c>
+      <c r="K52" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53">
+        <v>20045</v>
+      </c>
+      <c r="C53" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53">
+        <v>41331</v>
+      </c>
+      <c r="G53" t="s">
+        <v>48</v>
+      </c>
+      <c r="H53" s="2">
+        <v>42608</v>
+      </c>
+      <c r="I53" s="4">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="J53" t="s">
+        <v>150</v>
+      </c>
+      <c r="K53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54">
+        <v>83873</v>
+      </c>
+      <c r="C54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s">
+        <v>155</v>
+      </c>
+      <c r="G54" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55">
+        <v>83916</v>
+      </c>
+      <c r="C55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s">
+        <v>156</v>
+      </c>
+      <c r="G55" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56">
+        <v>83950</v>
+      </c>
+      <c r="C56" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" t="s">
+        <v>55</v>
+      </c>
+      <c r="I56" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57">
+        <v>83987</v>
+      </c>
+      <c r="C57" t="s">
+        <v>141</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" t="s">
+        <v>154</v>
+      </c>
+      <c r="G57" t="s">
+        <v>55</v>
+      </c>
+      <c r="I57" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58" t="s">
+        <v>164</v>
+      </c>
+      <c r="G58" t="s">
+        <v>55</v>
+      </c>
+      <c r="J58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" t="s">
+        <v>64</v>
+      </c>
+      <c r="E59" t="s">
+        <v>65</v>
+      </c>
+      <c r="F59">
+        <v>11347</v>
+      </c>
+      <c r="G59" t="s">
+        <v>55</v>
+      </c>
+      <c r="H59" s="2">
+        <v>42170</v>
+      </c>
+      <c r="I59" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J59" t="s">
+        <v>161</v>
+      </c>
+      <c r="K59" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:K38">
-    <sortCondition ref="A2:A38"/>
-    <sortCondition ref="B2:B38"/>
+  <sortState ref="A2:K59">
+    <sortCondition ref="A2:A59"/>
+    <sortCondition ref="B2:B59"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added items as they were packed away for Magnoia's visit
</commit_message>
<xml_diff>
--- a/trains/Inventory.xlsx
+++ b/trains/Inventory.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locomotives" sheetId="1" r:id="rId1"/>
     <sheet name="Rolling Stock" sheetId="2" r:id="rId2"/>
+    <sheet name="EZ Track" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="201">
   <si>
     <t>Road Name</t>
   </si>
@@ -538,6 +539,96 @@
   </si>
   <si>
     <t>70 ton flat car</t>
+  </si>
+  <si>
+    <t>40' wood milk car</t>
+  </si>
+  <si>
+    <t>Roundhouse</t>
+  </si>
+  <si>
+    <t>41' steel boxcar</t>
+  </si>
+  <si>
+    <t>Mantua</t>
+  </si>
+  <si>
+    <t>40' superior door boxcar</t>
+  </si>
+  <si>
+    <t>40' boxcar</t>
+  </si>
+  <si>
+    <t>50' PD Youngstown boxcar</t>
+  </si>
+  <si>
+    <t>Evans 4870 cu ft hopper</t>
+  </si>
+  <si>
+    <t>EE-1701-6</t>
+  </si>
+  <si>
+    <t>EMD GP7</t>
+  </si>
+  <si>
+    <t>actual price below sticker due to sale</t>
+  </si>
+  <si>
+    <t>Detrot &amp; Toledo Shore Line</t>
+  </si>
+  <si>
+    <t>ACF 60' DD auto parts car</t>
+  </si>
+  <si>
+    <t>1680-1</t>
+  </si>
+  <si>
+    <t>train show - Hub Division</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>26" radius curve</t>
+  </si>
+  <si>
+    <t>22" radius curve</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>18" radius curve</t>
+  </si>
+  <si>
+    <t>15" radius curve</t>
+  </si>
+  <si>
+    <t>9" straight</t>
+  </si>
+  <si>
+    <t>9" straight terminal</t>
+  </si>
+  <si>
+    <t>18" radius curve terminal</t>
+  </si>
+  <si>
+    <t>36" straight</t>
+  </si>
+  <si>
+    <t>30 degree crossover</t>
+  </si>
+  <si>
+    <t>remote turnout left</t>
+  </si>
+  <si>
+    <t>remote turnout right</t>
+  </si>
+  <si>
+    <t>Hayes bumper</t>
   </si>
 </sst>
 </file>
@@ -602,13 +693,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -947,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J6" sqref="A1:J6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1137,6 +1234,35 @@
         <v>124</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1575</v>
+      </c>
+      <c r="C7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>65605</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="4">
+        <v>112.95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:J6">
     <sortCondition ref="A2:A6"/>
@@ -1148,11 +1274,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="A1:K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,16 +1505,28 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>161</v>
+        <v>151</v>
+      </c>
+      <c r="C8" t="s">
+        <v>177</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>91264</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="I8" s="4">
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>127</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1396,31 +1534,16 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>462</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9">
-        <v>11350</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="2">
-        <v>42675</v>
-      </c>
-      <c r="I9" s="4">
-        <v>15.25</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1428,16 +1551,31 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>476</v>
+        <v>462</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10">
+        <v>11350</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="H10" s="2">
+        <v>42675</v>
+      </c>
+      <c r="I10" s="4">
+        <v>15.25</v>
       </c>
       <c r="J10" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1445,13 +1583,10 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>3204</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
+        <v>476</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>
@@ -1465,31 +1600,22 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>4587</v>
+        <v>1126</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F12">
-        <v>109050</v>
+        <v>70324</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2">
-        <v>42638</v>
-      </c>
-      <c r="I12" s="4">
-        <v>42.5</v>
-      </c>
-      <c r="J12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1497,31 +1623,28 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>4608</v>
+        <v>1923</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>172</v>
+      </c>
+      <c r="F13">
+        <v>84639</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="4">
         <v>18</v>
       </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13">
-        <v>109053</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="2">
-        <v>42638</v>
-      </c>
-      <c r="I13" s="4">
-        <v>42.5</v>
-      </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1529,28 +1652,19 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>5517</v>
+        <v>3204</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14">
-        <v>40931</v>
+        <v>129</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" s="4">
-        <v>18.95</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1558,25 +1672,31 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>5544</v>
+        <v>4587</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>21</v>
+      </c>
+      <c r="F15">
+        <v>109050</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
+        <v>19</v>
+      </c>
+      <c r="H15" s="2">
+        <v>42638</v>
       </c>
       <c r="I15" s="4">
-        <v>12</v>
+        <v>42.5</v>
       </c>
       <c r="J15" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1584,28 +1704,31 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>8900</v>
+        <v>4608</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F16">
-        <v>17644</v>
+        <v>109053</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>19</v>
+      </c>
+      <c r="H16" s="2">
+        <v>42638</v>
       </c>
       <c r="I16" s="4">
-        <v>12.95</v>
+        <v>42.5</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1613,31 +1736,28 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9061</v>
+        <v>5419</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17">
-        <v>913</v>
+        <v>81</v>
+      </c>
+      <c r="F17" t="s">
+        <v>179</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="I17" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
-      </c>
-      <c r="K17" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1645,31 +1765,28 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>9072</v>
+        <v>5517</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="F18">
-        <v>913</v>
+        <v>40931</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="I18" s="4">
-        <v>10</v>
+        <v>18.95</v>
       </c>
       <c r="J18" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1677,31 +1794,25 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>71729</v>
+        <v>5544</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
         <v>29</v>
       </c>
       <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="4">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="2">
-        <v>42305</v>
-      </c>
-      <c r="I19" s="4">
-        <v>4.8</v>
-      </c>
       <c r="J19" t="s">
-        <v>132</v>
-      </c>
-      <c r="K19" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1709,31 +1820,28 @@
         <v>16</v>
       </c>
       <c r="B20">
-        <v>71741</v>
+        <v>8900</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
         <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="F20">
+        <v>17644</v>
       </c>
       <c r="G20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="2">
-        <v>42305</v>
+        <v>48</v>
       </c>
       <c r="I20" s="4">
-        <v>4.8</v>
+        <v>12.95</v>
       </c>
       <c r="J20" t="s">
-        <v>132</v>
-      </c>
-      <c r="K20" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1741,28 +1849,31 @@
         <v>16</v>
       </c>
       <c r="B21">
-        <v>73035</v>
+        <v>9061</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" t="s">
-        <v>144</v>
+        <v>65</v>
+      </c>
+      <c r="F21">
+        <v>913</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="I21" s="4">
-        <v>25.95</v>
+        <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>145</v>
+        <v>59</v>
+      </c>
+      <c r="K21" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1770,31 +1881,31 @@
         <v>16</v>
       </c>
       <c r="B22">
-        <v>73060</v>
+        <v>9072</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" t="s">
-        <v>142</v>
+        <v>65</v>
+      </c>
+      <c r="F22">
+        <v>913</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="I22" s="4">
-        <v>29.95</v>
+        <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1802,13 +1913,13 @@
         <v>16</v>
       </c>
       <c r="B23">
-        <v>76032</v>
+        <v>71729</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1833,329 +1944,302 @@
       <c r="A24" t="s">
         <v>16</v>
       </c>
+      <c r="B24">
+        <v>71741</v>
+      </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24">
-        <v>18448</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>30</v>
+      </c>
+      <c r="H24" s="2">
+        <v>42305</v>
+      </c>
+      <c r="I24" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>132</v>
+      </c>
+      <c r="K24" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="B25">
-        <v>606902</v>
+        <v>73035</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25">
-        <v>19131</v>
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>144</v>
       </c>
       <c r="G25" t="s">
         <v>55</v>
       </c>
-      <c r="H25" s="2">
-        <v>42680</v>
-      </c>
       <c r="I25" s="4">
-        <v>10</v>
+        <v>25.95</v>
       </c>
       <c r="J25" t="s">
-        <v>61</v>
-      </c>
-      <c r="K25" t="s">
-        <v>62</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B26">
-        <v>2217</v>
+        <v>73060</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26">
-        <v>92893</v>
+        <v>53</v>
+      </c>
+      <c r="F26" t="s">
+        <v>142</v>
       </c>
       <c r="G26" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="2">
-        <v>42126</v>
-      </c>
       <c r="I26" s="4">
-        <v>15.98</v>
+        <v>29.95</v>
       </c>
       <c r="J26" t="s">
         <v>14</v>
       </c>
+      <c r="K26" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B27">
-        <v>3202</v>
+        <v>76032</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>55</v>
-      </c>
-      <c r="H27" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="H27" s="2">
+        <v>42305</v>
+      </c>
       <c r="I27" s="4">
-        <v>25.95</v>
+        <v>4.8</v>
       </c>
       <c r="J27" t="s">
-        <v>69</v>
+        <v>132</v>
+      </c>
+      <c r="K27" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B28">
-        <v>3226</v>
+        <v>77021</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" t="s">
-        <v>54</v>
+        <v>174</v>
+      </c>
+      <c r="F28">
+        <v>34530</v>
       </c>
       <c r="G28" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="2">
-        <v>42674</v>
+        <v>48</v>
       </c>
       <c r="I28" s="4">
-        <v>17</v>
+        <v>14.75</v>
       </c>
       <c r="J28" t="s">
-        <v>56</v>
-      </c>
-      <c r="K28" t="s">
-        <v>57</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B29">
-        <v>5006</v>
+        <v>77027</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" t="s">
-        <v>117</v>
+        <v>24</v>
+      </c>
+      <c r="F29">
+        <v>17048</v>
       </c>
       <c r="G29" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I29" s="4">
-        <v>15</v>
+        <v>12.95</v>
       </c>
       <c r="J29" t="s">
-        <v>118</v>
-      </c>
-      <c r="K29" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30">
-        <v>6128</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F30">
-        <v>97340</v>
+        <v>18448</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
-      </c>
-      <c r="I30" s="4">
-        <v>31.95</v>
-      </c>
-      <c r="J30" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31">
-        <v>1165</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" t="s">
-        <v>77</v>
-      </c>
-      <c r="F31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="B32">
-        <v>9602</v>
+        <v>606902</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F32">
-        <v>91487</v>
+        <v>19131</v>
       </c>
       <c r="G32" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H32" s="2">
-        <v>42309</v>
+        <v>42680</v>
       </c>
       <c r="I32" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J32" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="K32" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B33">
-        <v>9621</v>
+        <v>2217</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" t="s">
-        <v>86</v>
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>92893</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H33" s="2">
-        <v>42303</v>
+        <v>42126</v>
       </c>
       <c r="I33" s="4">
-        <v>29.95</v>
+        <v>15.98</v>
       </c>
       <c r="J33" t="s">
-        <v>93</v>
-      </c>
-      <c r="K33" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B34">
-        <v>10112</v>
+        <v>3202</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34">
-        <v>89082</v>
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>115</v>
       </c>
       <c r="G34" t="s">
-        <v>83</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H34" s="2"/>
       <c r="I34" s="4">
-        <v>27.98</v>
+        <v>25.95</v>
       </c>
       <c r="J34" t="s">
         <v>69</v>
@@ -2163,409 +2247,400 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B35">
-        <v>10312</v>
+        <v>3226</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35">
-        <v>17532</v>
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H35" s="2">
-        <v>42537</v>
+        <v>42674</v>
       </c>
       <c r="I35" s="4">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J35" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="K35" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B36">
-        <v>25907</v>
+        <v>5006</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F36" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="G36" t="s">
-        <v>83</v>
+        <v>48</v>
+      </c>
+      <c r="I36" s="4">
+        <v>15</v>
+      </c>
+      <c r="J36" t="s">
+        <v>118</v>
+      </c>
+      <c r="K36" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B37">
-        <v>32246</v>
+        <v>6128</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F37">
-        <v>18132</v>
+        <v>97340</v>
       </c>
       <c r="G37" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37" s="2">
-        <v>42411</v>
+        <v>88</v>
       </c>
       <c r="I37" s="4">
-        <v>12.5</v>
+        <v>31.95</v>
       </c>
       <c r="J37" t="s">
-        <v>91</v>
-      </c>
-      <c r="K37" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B38">
-        <v>113894</v>
+        <v>1165</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38">
-        <v>93725</v>
+        <v>77</v>
+      </c>
+      <c r="F38" t="s">
+        <v>78</v>
       </c>
       <c r="G38" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="2">
-        <v>42709</v>
-      </c>
-      <c r="I38" s="4">
-        <v>10</v>
-      </c>
-      <c r="J38" t="s">
-        <v>32</v>
-      </c>
-      <c r="K38" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B39">
-        <v>148077</v>
+        <v>9602</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="D39" t="s">
         <v>43</v>
       </c>
       <c r="E39" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>91487</v>
       </c>
       <c r="G39" t="s">
-        <v>30</v>
+        <v>48</v>
+      </c>
+      <c r="H39" s="2">
+        <v>42309</v>
       </c>
       <c r="I39" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J39" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B40">
-        <v>591263</v>
+        <v>9621</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="H40" s="2">
-        <v>42440</v>
+        <v>42303</v>
       </c>
       <c r="I40" s="4">
-        <v>14.99</v>
+        <v>29.95</v>
       </c>
       <c r="J40" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="K40" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B41">
-        <v>598016</v>
+        <v>10112</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
       </c>
       <c r="F41">
-        <v>92957</v>
+        <v>89082</v>
       </c>
       <c r="G41" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="2">
-        <v>42680</v>
+        <v>83</v>
       </c>
       <c r="I41" s="4">
-        <v>14</v>
+        <v>27.98</v>
       </c>
       <c r="J41" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B42">
-        <v>675097</v>
+        <v>10312</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
-      </c>
-      <c r="F42" t="s">
-        <v>39</v>
+        <v>24</v>
+      </c>
+      <c r="F42">
+        <v>17532</v>
       </c>
       <c r="G42" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="H42" s="2">
-        <v>42521</v>
+        <v>42537</v>
       </c>
       <c r="I42" s="4">
-        <v>16.489999999999998</v>
+        <v>11</v>
       </c>
       <c r="J42" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="K42" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B43">
-        <v>2706</v>
+        <v>25907</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43">
-        <v>92912</v>
+        <v>81</v>
+      </c>
+      <c r="F43" t="s">
+        <v>82</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="2">
-        <v>42637</v>
-      </c>
-      <c r="I43" s="4">
-        <v>13.29</v>
-      </c>
-      <c r="J43" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B44">
-        <v>14274</v>
+        <v>32246</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F44">
-        <v>5648</v>
+        <v>18132</v>
       </c>
       <c r="G44" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H44" s="2">
-        <v>42672</v>
+        <v>42411</v>
       </c>
       <c r="I44" s="4">
-        <v>7</v>
+        <v>12.5</v>
       </c>
       <c r="J44" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="K44" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>182</v>
       </c>
       <c r="B45">
-        <v>14450</v>
+        <v>5546</v>
       </c>
       <c r="C45" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="D45" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45">
-        <v>5648</v>
+        <v>65</v>
+      </c>
+      <c r="F45" t="s">
+        <v>184</v>
       </c>
       <c r="G45" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H45" s="2">
-        <v>42672</v>
+        <v>42708</v>
       </c>
       <c r="I45" s="4">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J45" t="s">
-        <v>49</v>
-      </c>
-      <c r="K45" t="s">
-        <v>67</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B46">
-        <v>16534</v>
+        <v>113894</v>
       </c>
       <c r="C46" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="E46" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" t="s">
-        <v>158</v>
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>93725</v>
       </c>
       <c r="G46" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="H46" s="2">
+        <v>42709</v>
+      </c>
+      <c r="I46" s="4">
+        <v>10</v>
       </c>
       <c r="J46" t="s">
-        <v>159</v>
+        <v>32</v>
+      </c>
+      <c r="K46" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B47">
-        <v>18878</v>
+        <v>148077</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="D47" t="s">
         <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="I47" s="4">
+        <v>12</v>
       </c>
       <c r="J47" t="s">
         <v>45</v>
@@ -2573,115 +2648,136 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B48">
-        <v>18881</v>
+        <v>591263</v>
       </c>
       <c r="C48" t="s">
-        <v>152</v>
+        <v>33</v>
       </c>
       <c r="D48" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="F48" t="s">
-        <v>167</v>
+        <v>35</v>
       </c>
       <c r="G48" t="s">
-        <v>48</v>
+        <v>13</v>
+      </c>
+      <c r="H48" s="2">
+        <v>42440</v>
+      </c>
+      <c r="I48" s="4">
+        <v>14.99</v>
       </c>
       <c r="J48" t="s">
-        <v>45</v>
+        <v>36</v>
+      </c>
+      <c r="K48" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B49">
-        <v>18914</v>
+        <v>598016</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F49" t="s">
-        <v>168</v>
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <v>92957</v>
       </c>
       <c r="G49" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="H49" s="2">
+        <v>42680</v>
+      </c>
+      <c r="I49" s="4">
+        <v>14</v>
       </c>
       <c r="J49" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B50">
-        <v>18942</v>
+        <v>675097</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E50" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="F50" t="s">
-        <v>169</v>
+        <v>39</v>
       </c>
       <c r="G50" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="H50" s="2">
+        <v>42521</v>
+      </c>
+      <c r="I50" s="4">
+        <v>16.489999999999998</v>
       </c>
       <c r="J50" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="K50" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B51">
-        <v>20025</v>
+        <v>2706</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="F51">
-        <v>41329</v>
+        <v>92912</v>
       </c>
       <c r="G51" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H51" s="2">
-        <v>42608</v>
+        <v>42637</v>
       </c>
       <c r="I51" s="4">
-        <v>17.989999999999998</v>
+        <v>13.29</v>
       </c>
       <c r="J51" t="s">
-        <v>150</v>
-      </c>
-      <c r="K51" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2689,34 +2785,34 @@
         <v>47</v>
       </c>
       <c r="B52">
-        <v>20037</v>
+        <v>14274</v>
       </c>
       <c r="C52" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="D52" t="s">
         <v>29</v>
       </c>
       <c r="E52" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="F52">
-        <v>41330</v>
+        <v>5648</v>
       </c>
       <c r="G52" t="s">
         <v>48</v>
       </c>
       <c r="H52" s="2">
-        <v>42608</v>
+        <v>42672</v>
       </c>
       <c r="I52" s="4">
-        <v>17.989999999999998</v>
+        <v>7</v>
       </c>
       <c r="J52" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="K52" t="s">
-        <v>151</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2724,34 +2820,34 @@
         <v>47</v>
       </c>
       <c r="B53">
-        <v>20045</v>
+        <v>14450</v>
       </c>
       <c r="C53" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="D53" t="s">
         <v>29</v>
       </c>
       <c r="E53" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="F53">
-        <v>41331</v>
+        <v>5648</v>
       </c>
       <c r="G53" t="s">
         <v>48</v>
       </c>
       <c r="H53" s="2">
-        <v>42608</v>
+        <v>42672</v>
       </c>
       <c r="I53" s="4">
-        <v>17.989999999999998</v>
+        <v>7</v>
       </c>
       <c r="J53" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="K53" t="s">
-        <v>151</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2759,28 +2855,25 @@
         <v>47</v>
       </c>
       <c r="B54">
-        <v>83873</v>
+        <v>16534</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
       <c r="E54" t="s">
         <v>53</v>
       </c>
       <c r="F54" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G54" t="s">
-        <v>55</v>
-      </c>
-      <c r="I54" s="4">
-        <v>23.95</v>
+        <v>48</v>
       </c>
       <c r="J54" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2788,28 +2881,25 @@
         <v>47</v>
       </c>
       <c r="B55">
-        <v>83916</v>
+        <v>18878</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="F55" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="G55" t="s">
-        <v>55</v>
-      </c>
-      <c r="I55" s="4">
-        <v>23.95</v>
+        <v>48</v>
       </c>
       <c r="J55" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2817,28 +2907,25 @@
         <v>47</v>
       </c>
       <c r="B56">
-        <v>83950</v>
+        <v>18881</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="F56" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="G56" t="s">
-        <v>55</v>
-      </c>
-      <c r="I56" s="4">
-        <v>23.95</v>
+        <v>48</v>
       </c>
       <c r="J56" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2846,97 +2933,464 @@
         <v>47</v>
       </c>
       <c r="B57">
-        <v>83987</v>
+        <v>18914</v>
       </c>
       <c r="C57" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E57" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="F57" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="G57" t="s">
-        <v>55</v>
-      </c>
-      <c r="I57" s="4">
-        <v>23.95</v>
+        <v>48</v>
       </c>
       <c r="J57" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>47</v>
       </c>
-      <c r="B58" t="s">
-        <v>162</v>
+      <c r="B58">
+        <v>18942</v>
       </c>
       <c r="C58" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D58" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="E58" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="F58" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G58" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J58" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>47</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59">
+        <v>20025</v>
+      </c>
+      <c r="C59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59">
+        <v>41329</v>
+      </c>
+      <c r="G59" t="s">
+        <v>48</v>
+      </c>
+      <c r="H59" s="2">
+        <v>42608</v>
+      </c>
+      <c r="I59" s="4">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="J59" t="s">
+        <v>150</v>
+      </c>
+      <c r="K59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60">
+        <v>20037</v>
+      </c>
+      <c r="C60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" t="s">
+        <v>29</v>
+      </c>
+      <c r="E60" t="s">
+        <v>140</v>
+      </c>
+      <c r="F60">
+        <v>41330</v>
+      </c>
+      <c r="G60" t="s">
+        <v>48</v>
+      </c>
+      <c r="H60" s="2">
+        <v>42608</v>
+      </c>
+      <c r="I60" s="4">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="J60" t="s">
+        <v>150</v>
+      </c>
+      <c r="K60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61">
+        <v>20045</v>
+      </c>
+      <c r="C61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" t="s">
+        <v>29</v>
+      </c>
+      <c r="E61" t="s">
+        <v>140</v>
+      </c>
+      <c r="F61">
+        <v>41331</v>
+      </c>
+      <c r="G61" t="s">
+        <v>48</v>
+      </c>
+      <c r="H61" s="2">
+        <v>42608</v>
+      </c>
+      <c r="I61" s="4">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="J61" t="s">
+        <v>150</v>
+      </c>
+      <c r="K61" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62">
+        <v>83873</v>
+      </c>
+      <c r="C62" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62" t="s">
+        <v>155</v>
+      </c>
+      <c r="G62" t="s">
+        <v>55</v>
+      </c>
+      <c r="I62" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J62" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63">
+        <v>83916</v>
+      </c>
+      <c r="C63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" t="s">
+        <v>53</v>
+      </c>
+      <c r="F63" t="s">
+        <v>156</v>
+      </c>
+      <c r="G63" t="s">
+        <v>55</v>
+      </c>
+      <c r="I63" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J63" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64">
+        <v>83950</v>
+      </c>
+      <c r="C64" t="s">
+        <v>141</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>53</v>
+      </c>
+      <c r="F64" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" t="s">
+        <v>55</v>
+      </c>
+      <c r="I64" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65">
+        <v>83987</v>
+      </c>
+      <c r="C65" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>53</v>
+      </c>
+      <c r="F65" t="s">
+        <v>154</v>
+      </c>
+      <c r="G65" t="s">
+        <v>55</v>
+      </c>
+      <c r="I65" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66" t="s">
+        <v>163</v>
+      </c>
+      <c r="D66" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" t="s">
+        <v>164</v>
+      </c>
+      <c r="G66" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" t="s">
         <v>160</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C67" t="s">
         <v>63</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D67" t="s">
         <v>64</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E67" t="s">
         <v>65</v>
       </c>
-      <c r="F59">
+      <c r="F67">
         <v>11347</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G67" t="s">
         <v>55</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H67" s="2">
         <v>42170</v>
       </c>
-      <c r="I59" s="4">
+      <c r="I67" s="4">
         <v>21.5</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J67" t="s">
         <v>161</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K67" t="s">
         <v>165</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K59">
-    <sortCondition ref="A2:A59"/>
-    <sortCondition ref="B2:B59"/>
+  <sortState ref="A2:K67">
+    <sortCondition ref="A2:A67"/>
+    <sortCondition ref="B2:B67"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
B&M boxcar from train show in Pepperell
</commit_message>
<xml_diff>
--- a/trains/Inventory.xlsx
+++ b/trains/Inventory.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="252">
   <si>
     <t>Road Name</t>
   </si>
@@ -731,9 +731,6 @@
     <t>Grank Trunk</t>
   </si>
   <si>
-    <t>any</t>
-  </si>
-  <si>
     <t>50' FMC plug door boxcar</t>
   </si>
   <si>
@@ -753,6 +750,39 @@
   </si>
   <si>
     <t>20 002 921</t>
+  </si>
+  <si>
+    <t>NACC 8K beer can tank</t>
+  </si>
+  <si>
+    <t>%30 off sale</t>
+  </si>
+  <si>
+    <t>Soo Line</t>
+  </si>
+  <si>
+    <t>932-7956</t>
+  </si>
+  <si>
+    <t>clearance sale</t>
+  </si>
+  <si>
+    <t>Michigan Central</t>
+  </si>
+  <si>
+    <t>http://www.modeltrainstuff.com/Athearn-HO-73518-40-Box-Car-MC-p/ath-73518.htm</t>
+  </si>
+  <si>
+    <t>https://www.lombardhobby.com/Athearn-RTR-Wide-Vision-Caboose-p/ath74143.htm</t>
+  </si>
+  <si>
+    <t>http://www.atlasrr.com/HOFreight/hocylin2.htm</t>
+  </si>
+  <si>
+    <t>50' FMC boxcar</t>
+  </si>
+  <si>
+    <t>train show - Pepperell</t>
   </si>
 </sst>
 </file>
@@ -1407,11 +1437,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1588,28 +1618,37 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>104</v>
       </c>
       <c r="B6">
-        <v>527</v>
+        <v>78376</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>241</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>218</v>
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>89138</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>82</v>
+      </c>
+      <c r="H6" s="2">
+        <v>42854</v>
       </c>
       <c r="I6" s="4">
-        <v>17</v>
+        <v>24.53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1617,34 +1656,25 @@
         <v>210</v>
       </c>
       <c r="B7">
-        <v>615</v>
+        <v>527</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <v>7159</v>
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>218</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="2">
-        <v>42245</v>
+        <v>87</v>
       </c>
       <c r="I7" s="4">
-        <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>217</v>
-      </c>
-      <c r="K7" t="s">
-        <v>216</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1652,34 +1682,34 @@
         <v>210</v>
       </c>
       <c r="B8">
-        <v>1233</v>
+        <v>615</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>221</v>
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>7159</v>
       </c>
       <c r="G8" t="s">
         <v>71</v>
       </c>
       <c r="H8" s="2">
-        <v>42204</v>
+        <v>42245</v>
       </c>
       <c r="I8" s="4">
-        <v>15.95</v>
+        <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1687,7 +1717,7 @@
         <v>210</v>
       </c>
       <c r="B9">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C9" t="s">
         <v>214</v>
@@ -1696,25 +1726,25 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F9">
-        <v>5214</v>
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>221</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="H9" s="2">
-        <v>42299</v>
+        <v>42204</v>
       </c>
       <c r="I9" s="4">
-        <v>19.95</v>
+        <v>15.95</v>
       </c>
       <c r="J9" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="K9" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1722,49 +1752,63 @@
         <v>210</v>
       </c>
       <c r="B10">
-        <v>2032</v>
+        <v>1234</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>207</v>
       </c>
       <c r="F10">
-        <v>21400</v>
+        <v>5214</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="H10" s="2">
+        <v>42299</v>
       </c>
       <c r="I10" s="4">
-        <v>10</v>
+        <v>19.95</v>
       </c>
       <c r="J10" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="K10" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>210</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2032</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11">
+        <v>21400</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="I11" s="4">
+        <v>10</v>
+      </c>
       <c r="J11" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1772,25 +1816,20 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="4">
-        <v>15</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="H12" s="2"/>
       <c r="J12" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1798,19 +1837,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>91264</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
         <v>30</v>
@@ -1819,7 +1855,7 @@
         <v>15</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1827,16 +1863,28 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>161</v>
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>176</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>91264</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="I14" s="4">
+        <v>15</v>
       </c>
       <c r="J14" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1844,31 +1892,16 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>462</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15">
-        <v>11350</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="2">
-        <v>42675</v>
-      </c>
-      <c r="I15" s="4">
-        <v>15.25</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1876,16 +1909,31 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>476</v>
+        <v>462</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>11350</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="H16" s="2">
+        <v>42675</v>
+      </c>
+      <c r="I16" s="4">
+        <v>15.25</v>
       </c>
       <c r="J16" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1893,22 +1941,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1126</v>
-      </c>
-      <c r="C17" t="s">
-        <v>174</v>
+        <v>476</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17">
-        <v>70324</v>
+        <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="J17" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1916,28 +1958,22 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1923</v>
+        <v>1126</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="F18">
-        <v>84639</v>
+        <v>70324</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="4">
-        <v>18</v>
-      </c>
-      <c r="J18" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1945,19 +1981,28 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>3204</v>
+        <v>1923</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19">
+        <v>84639</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="I19" s="4">
+        <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1965,31 +2010,19 @@
         <v>16</v>
       </c>
       <c r="B20">
-        <v>4587</v>
+        <v>3204</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20">
-        <v>109050</v>
+        <v>128</v>
       </c>
       <c r="G20" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="2">
-        <v>42638</v>
-      </c>
-      <c r="I20" s="4">
-        <v>42.5</v>
-      </c>
       <c r="J20" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1997,7 +2030,7 @@
         <v>16</v>
       </c>
       <c r="B21">
-        <v>4608</v>
+        <v>4587</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -2009,7 +2042,7 @@
         <v>21</v>
       </c>
       <c r="F21">
-        <v>109053</v>
+        <v>109050</v>
       </c>
       <c r="G21" t="s">
         <v>19</v>
@@ -2029,28 +2062,31 @@
         <v>16</v>
       </c>
       <c r="B22">
-        <v>5419</v>
+        <v>4608</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" t="s">
-        <v>178</v>
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>109053</v>
       </c>
       <c r="G22" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="H22" s="2">
+        <v>42638</v>
       </c>
       <c r="I22" s="4">
-        <v>26</v>
+        <v>42.5</v>
       </c>
       <c r="J22" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -2058,28 +2094,28 @@
         <v>16</v>
       </c>
       <c r="B23">
-        <v>5517</v>
+        <v>5419</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="D23" t="s">
         <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
-      </c>
-      <c r="F23">
-        <v>40931</v>
+        <v>80</v>
+      </c>
+      <c r="F23" t="s">
+        <v>178</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="I23" s="4">
-        <v>18.95</v>
+        <v>26</v>
       </c>
       <c r="J23" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -2087,22 +2123,25 @@
         <v>16</v>
       </c>
       <c r="B24">
-        <v>5544</v>
+        <v>5517</v>
       </c>
       <c r="C24" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
         <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>139</v>
+      </c>
+      <c r="F24">
+        <v>40931</v>
       </c>
       <c r="G24" t="s">
         <v>87</v>
       </c>
       <c r="I24" s="4">
-        <v>12</v>
+        <v>18.95</v>
       </c>
       <c r="J24" t="s">
         <v>45</v>
@@ -2113,34 +2152,25 @@
         <v>16</v>
       </c>
       <c r="B25">
-        <v>7509</v>
+        <v>5544</v>
       </c>
       <c r="C25" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
       <c r="D25" t="s">
         <v>29</v>
       </c>
       <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="4">
         <v>12</v>
       </c>
-      <c r="F25">
-        <v>76483</v>
-      </c>
-      <c r="G25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" s="8">
-        <v>42785</v>
-      </c>
-      <c r="I25" s="4">
-        <v>34.979999999999997</v>
-      </c>
       <c r="J25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" t="s">
-        <v>205</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -2148,28 +2178,34 @@
         <v>16</v>
       </c>
       <c r="B26">
-        <v>8900</v>
+        <v>7509</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="D26" t="s">
         <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26">
-        <v>17644</v>
+        <v>76483</v>
       </c>
       <c r="G26" t="s">
         <v>48</v>
       </c>
+      <c r="H26" s="8">
+        <v>42785</v>
+      </c>
       <c r="I26" s="4">
-        <v>12.95</v>
+        <v>34.979999999999997</v>
       </c>
       <c r="J26" t="s">
-        <v>68</v>
+        <v>14</v>
+      </c>
+      <c r="K26" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -2177,31 +2213,28 @@
         <v>16</v>
       </c>
       <c r="B27">
-        <v>9061</v>
+        <v>8900</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>913</v>
+        <v>17644</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="I27" s="4">
-        <v>10</v>
+        <v>12.95</v>
       </c>
       <c r="J27" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27" t="s">
-        <v>146</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -2209,7 +2242,7 @@
         <v>16</v>
       </c>
       <c r="B28">
-        <v>9072</v>
+        <v>9061</v>
       </c>
       <c r="C28" t="s">
         <v>145</v>
@@ -2241,31 +2274,31 @@
         <v>16</v>
       </c>
       <c r="B29">
-        <v>71729</v>
+        <v>9072</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>64</v>
+      </c>
+      <c r="F29">
+        <v>913</v>
       </c>
       <c r="G29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="2">
-        <v>42305</v>
+        <v>71</v>
       </c>
       <c r="I29" s="4">
-        <v>4.8</v>
+        <v>10</v>
       </c>
       <c r="J29" t="s">
-        <v>131</v>
+        <v>58</v>
       </c>
       <c r="K29" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -2273,7 +2306,7 @@
         <v>16</v>
       </c>
       <c r="B30">
-        <v>71741</v>
+        <v>71729</v>
       </c>
       <c r="C30" t="s">
         <v>130</v>
@@ -2305,28 +2338,31 @@
         <v>16</v>
       </c>
       <c r="B31">
-        <v>73035</v>
+        <v>71741</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>30</v>
+      </c>
+      <c r="H31" s="2">
+        <v>42305</v>
       </c>
       <c r="I31" s="4">
-        <v>25.95</v>
+        <v>4.8</v>
       </c>
       <c r="J31" t="s">
-        <v>144</v>
+        <v>131</v>
+      </c>
+      <c r="K31" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -2334,7 +2370,7 @@
         <v>16</v>
       </c>
       <c r="B32">
-        <v>73060</v>
+        <v>73035</v>
       </c>
       <c r="C32" t="s">
         <v>140</v>
@@ -2346,19 +2382,16 @@
         <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G32" t="s">
         <v>55</v>
       </c>
       <c r="I32" s="4">
-        <v>29.95</v>
+        <v>25.95</v>
       </c>
       <c r="J32" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2366,31 +2399,31 @@
         <v>16</v>
       </c>
       <c r="B33">
-        <v>76032</v>
+        <v>73060</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>53</v>
+      </c>
+      <c r="F33" t="s">
+        <v>141</v>
       </c>
       <c r="G33" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="2">
-        <v>42305</v>
+        <v>55</v>
       </c>
       <c r="I33" s="4">
-        <v>4.8</v>
+        <v>29.95</v>
       </c>
       <c r="J33" t="s">
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="K33" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2398,28 +2431,31 @@
         <v>16</v>
       </c>
       <c r="B34">
-        <v>77021</v>
+        <v>76032</v>
       </c>
       <c r="C34" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>173</v>
-      </c>
-      <c r="F34">
-        <v>34530</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="H34" s="2">
+        <v>42305</v>
       </c>
       <c r="I34" s="4">
-        <v>14.75</v>
+        <v>4.8</v>
       </c>
       <c r="J34" t="s">
-        <v>158</v>
+        <v>131</v>
+      </c>
+      <c r="K34" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -2427,120 +2463,144 @@
         <v>16</v>
       </c>
       <c r="B35">
-        <v>77027</v>
+        <v>77021</v>
       </c>
       <c r="C35" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="F35">
-        <v>17048</v>
+        <v>34530</v>
       </c>
       <c r="G35" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="I35" s="4">
-        <v>12.95</v>
+        <v>14.75</v>
       </c>
       <c r="J35" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>16</v>
       </c>
+      <c r="B36">
+        <v>77027</v>
+      </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
         <v>24</v>
       </c>
       <c r="F36">
-        <v>18448</v>
+        <v>17048</v>
       </c>
       <c r="G36" t="s">
-        <v>55</v>
+        <v>30</v>
+      </c>
+      <c r="I36" s="4">
+        <v>12.95</v>
+      </c>
+      <c r="J36" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>16</v>
       </c>
+      <c r="B37">
+        <v>80014</v>
+      </c>
+      <c r="C37" t="s">
+        <v>250</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <v>92513</v>
+      </c>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="2">
+        <v>43009</v>
+      </c>
+      <c r="I37" s="4">
+        <v>10</v>
+      </c>
+      <c r="J37" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>129</v>
-      </c>
-      <c r="B38">
-        <v>606902</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
         <v>24</v>
       </c>
       <c r="F38">
-        <v>19131</v>
+        <v>18448</v>
       </c>
       <c r="G38" t="s">
         <v>55</v>
       </c>
-      <c r="H38" s="2">
-        <v>42680</v>
-      </c>
-      <c r="I38" s="4">
-        <v>10</v>
-      </c>
-      <c r="J38" t="s">
-        <v>60</v>
-      </c>
-      <c r="K38" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B39">
-        <v>2217</v>
+        <v>606902</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F39">
-        <v>92893</v>
+        <v>19131</v>
       </c>
       <c r="G39" t="s">
         <v>55</v>
       </c>
       <c r="H39" s="2">
-        <v>42126</v>
+        <v>42680</v>
       </c>
       <c r="I39" s="4">
-        <v>15.98</v>
+        <v>10</v>
       </c>
       <c r="J39" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="K39" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2548,29 +2608,31 @@
         <v>51</v>
       </c>
       <c r="B40">
-        <v>3202</v>
+        <v>2217</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
-      </c>
-      <c r="F40" t="s">
-        <v>114</v>
+        <v>12</v>
+      </c>
+      <c r="F40">
+        <v>92893</v>
       </c>
       <c r="G40" t="s">
         <v>55</v>
       </c>
-      <c r="H40" s="2"/>
+      <c r="H40" s="2">
+        <v>42126</v>
+      </c>
       <c r="I40" s="4">
-        <v>25.95</v>
+        <v>15.98</v>
       </c>
       <c r="J40" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2578,7 +2640,7 @@
         <v>51</v>
       </c>
       <c r="B41">
-        <v>3226</v>
+        <v>3202</v>
       </c>
       <c r="C41" t="s">
         <v>52</v>
@@ -2590,22 +2652,17 @@
         <v>53</v>
       </c>
       <c r="F41" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="G41" t="s">
         <v>55</v>
       </c>
-      <c r="H41" s="2">
-        <v>42674</v>
-      </c>
+      <c r="H41" s="2"/>
       <c r="I41" s="4">
-        <v>17</v>
+        <v>25.95</v>
       </c>
       <c r="J41" t="s">
-        <v>56</v>
-      </c>
-      <c r="K41" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2613,31 +2670,34 @@
         <v>51</v>
       </c>
       <c r="B42">
-        <v>5006</v>
+        <v>3226</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F42" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="G42" t="s">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="H42" s="2">
+        <v>42674</v>
       </c>
       <c r="I42" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J42" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="K42" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2645,63 +2705,60 @@
         <v>51</v>
       </c>
       <c r="B43">
-        <v>6128</v>
+        <v>5006</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
         <v>29</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43">
-        <v>97340</v>
+        <v>64</v>
+      </c>
+      <c r="F43" t="s">
+        <v>116</v>
       </c>
       <c r="G43" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="I43" s="4">
-        <v>31.95</v>
+        <v>15</v>
       </c>
       <c r="J43" t="s">
-        <v>68</v>
+        <v>117</v>
+      </c>
+      <c r="K43" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B44">
-        <v>133</v>
+        <v>6128</v>
       </c>
       <c r="C44" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="D44" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E44" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="F44">
-        <v>76832</v>
+        <v>97340</v>
       </c>
       <c r="G44" t="s">
-        <v>55</v>
-      </c>
-      <c r="H44" s="2">
-        <v>42770</v>
+        <v>87</v>
       </c>
       <c r="I44" s="4">
-        <v>26.98</v>
+        <v>31.95</v>
       </c>
       <c r="J44" t="s">
-        <v>14</v>
-      </c>
-      <c r="K44" t="s">
-        <v>201</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -2709,22 +2766,34 @@
         <v>73</v>
       </c>
       <c r="B45">
-        <v>1165</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>200</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E45" t="s">
-        <v>76</v>
-      </c>
-      <c r="F45" t="s">
-        <v>77</v>
+        <v>171</v>
+      </c>
+      <c r="F45">
+        <v>76832</v>
       </c>
       <c r="G45" t="s">
-        <v>78</v>
+        <v>55</v>
+      </c>
+      <c r="H45" s="2">
+        <v>42770</v>
+      </c>
+      <c r="I45" s="4">
+        <v>26.98</v>
+      </c>
+      <c r="J45" t="s">
+        <v>14</v>
+      </c>
+      <c r="K45" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2732,31 +2801,22 @@
         <v>73</v>
       </c>
       <c r="B46">
-        <v>9602</v>
+        <v>1165</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46">
-        <v>91487</v>
+        <v>76</v>
+      </c>
+      <c r="F46" t="s">
+        <v>77</v>
       </c>
       <c r="G46" t="s">
-        <v>48</v>
-      </c>
-      <c r="H46" s="2">
-        <v>42309</v>
-      </c>
-      <c r="I46" s="4">
-        <v>16</v>
-      </c>
-      <c r="J46" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2764,34 +2824,31 @@
         <v>73</v>
       </c>
       <c r="B47">
-        <v>9621</v>
+        <v>9602</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D47" t="s">
         <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" t="s">
-        <v>85</v>
+        <v>12</v>
+      </c>
+      <c r="F47">
+        <v>91487</v>
       </c>
       <c r="G47" t="s">
         <v>48</v>
       </c>
       <c r="H47" s="2">
-        <v>42303</v>
+        <v>42309</v>
       </c>
       <c r="I47" s="4">
-        <v>29.95</v>
+        <v>16</v>
       </c>
       <c r="J47" t="s">
-        <v>92</v>
-      </c>
-      <c r="K47" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -2799,28 +2856,34 @@
         <v>73</v>
       </c>
       <c r="B48">
-        <v>10112</v>
+        <v>9621</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48">
-        <v>89082</v>
+        <v>80</v>
+      </c>
+      <c r="F48" t="s">
+        <v>85</v>
       </c>
       <c r="G48" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+      <c r="H48" s="2">
+        <v>42303</v>
       </c>
       <c r="I48" s="4">
-        <v>27.98</v>
+        <v>29.95</v>
       </c>
       <c r="J48" t="s">
-        <v>68</v>
+        <v>92</v>
+      </c>
+      <c r="K48" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2828,34 +2891,28 @@
         <v>73</v>
       </c>
       <c r="B49">
-        <v>10312</v>
+        <v>10112</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D49" t="s">
         <v>29</v>
       </c>
       <c r="E49" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F49">
-        <v>17532</v>
+        <v>89082</v>
       </c>
       <c r="G49" t="s">
-        <v>87</v>
-      </c>
-      <c r="H49" s="2">
-        <v>42537</v>
+        <v>82</v>
       </c>
       <c r="I49" s="4">
-        <v>11</v>
+        <v>27.98</v>
       </c>
       <c r="J49" t="s">
-        <v>88</v>
-      </c>
-      <c r="K49" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2863,22 +2920,34 @@
         <v>73</v>
       </c>
       <c r="B50">
-        <v>25907</v>
+        <v>10312</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50">
+        <v>17532</v>
+      </c>
+      <c r="G50" t="s">
+        <v>87</v>
+      </c>
+      <c r="H50" s="2">
+        <v>42537</v>
+      </c>
+      <c r="I50" s="4">
         <v>11</v>
       </c>
-      <c r="E50" t="s">
-        <v>80</v>
-      </c>
-      <c r="F50" t="s">
-        <v>81</v>
-      </c>
-      <c r="G50" t="s">
-        <v>82</v>
+      <c r="J50" t="s">
+        <v>88</v>
+      </c>
+      <c r="K50" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2886,98 +2955,89 @@
         <v>73</v>
       </c>
       <c r="B51">
-        <v>32246</v>
+        <v>25907</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51">
-        <v>18132</v>
+        <v>80</v>
+      </c>
+      <c r="F51" t="s">
+        <v>81</v>
       </c>
       <c r="G51" t="s">
-        <v>30</v>
-      </c>
-      <c r="H51" s="2">
-        <v>42411</v>
-      </c>
-      <c r="I51" s="4">
-        <v>12.5</v>
-      </c>
-      <c r="J51" t="s">
-        <v>90</v>
-      </c>
-      <c r="K51" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="B52">
-        <v>5546</v>
+        <v>32246</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
+        <v>83</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>64</v>
-      </c>
-      <c r="F52" t="s">
-        <v>183</v>
+        <v>24</v>
+      </c>
+      <c r="F52">
+        <v>18132</v>
       </c>
       <c r="G52" t="s">
         <v>30</v>
       </c>
       <c r="H52" s="2">
-        <v>42708</v>
+        <v>42411</v>
       </c>
       <c r="I52" s="4">
-        <v>18</v>
+        <v>12.5</v>
       </c>
       <c r="J52" t="s">
-        <v>184</v>
+        <v>90</v>
+      </c>
+      <c r="K52" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="B53">
-        <v>112115</v>
+        <v>5546</v>
       </c>
       <c r="C53" t="s">
-        <v>236</v>
+        <v>182</v>
       </c>
       <c r="D53" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
         <v>64</v>
       </c>
       <c r="F53" t="s">
-        <v>237</v>
+        <v>183</v>
       </c>
       <c r="G53" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H53" s="2">
-        <v>46500</v>
+        <v>42708</v>
       </c>
       <c r="I53" s="4">
-        <v>13.6</v>
+        <v>18</v>
       </c>
       <c r="J53" t="s">
-        <v>238</v>
+        <v>184</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2985,10 +3045,10 @@
         <v>22</v>
       </c>
       <c r="B54">
-        <v>112143</v>
+        <v>112115</v>
       </c>
       <c r="C54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D54" t="s">
         <v>29</v>
@@ -2997,22 +3057,19 @@
         <v>64</v>
       </c>
       <c r="F54" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G54" t="s">
         <v>19</v>
       </c>
       <c r="H54" s="2">
-        <v>42793</v>
+        <v>46500</v>
       </c>
       <c r="I54" s="4">
-        <v>18</v>
+        <v>13.6</v>
       </c>
       <c r="J54" t="s">
-        <v>239</v>
-      </c>
-      <c r="K54" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -3020,34 +3077,34 @@
         <v>22</v>
       </c>
       <c r="B55">
-        <v>113894</v>
+        <v>112143</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
         <v>29</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55">
-        <v>93725</v>
+        <v>64</v>
+      </c>
+      <c r="F55" t="s">
+        <v>240</v>
       </c>
       <c r="G55" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H55" s="2">
-        <v>42709</v>
+        <v>42793</v>
       </c>
       <c r="I55" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="J55" t="s">
-        <v>32</v>
+        <v>238</v>
       </c>
       <c r="K55" t="s">
-        <v>31</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -3055,25 +3112,34 @@
         <v>22</v>
       </c>
       <c r="B56">
-        <v>148077</v>
+        <v>113894</v>
       </c>
       <c r="C56" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>93725</v>
       </c>
       <c r="G56" t="s">
         <v>30</v>
       </c>
+      <c r="H56" s="2">
+        <v>42709</v>
+      </c>
       <c r="I56" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J56" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="K56" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -3081,34 +3147,25 @@
         <v>22</v>
       </c>
       <c r="B57">
-        <v>591263</v>
+        <v>148077</v>
       </c>
       <c r="C57" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E57" t="s">
-        <v>34</v>
-      </c>
-      <c r="F57" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G57" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="2">
-        <v>42440</v>
+        <v>30</v>
       </c>
       <c r="I57" s="4">
-        <v>14.99</v>
+        <v>12</v>
       </c>
       <c r="J57" t="s">
-        <v>36</v>
-      </c>
-      <c r="K57" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -3116,31 +3173,34 @@
         <v>22</v>
       </c>
       <c r="B58">
-        <v>598016</v>
+        <v>591263</v>
       </c>
       <c r="C58" t="s">
-        <v>235</v>
+        <v>33</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58">
-        <v>92957</v>
+        <v>34</v>
+      </c>
+      <c r="F58" t="s">
+        <v>35</v>
       </c>
       <c r="G58" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H58" s="2">
-        <v>42680</v>
+        <v>42440</v>
       </c>
       <c r="I58" s="4">
-        <v>14</v>
+        <v>14.99</v>
       </c>
       <c r="J58" t="s">
-        <v>58</v>
+        <v>36</v>
+      </c>
+      <c r="K58" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -3148,101 +3208,98 @@
         <v>22</v>
       </c>
       <c r="B59">
-        <v>675097</v>
+        <v>598016</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="D59" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E59" t="s">
-        <v>34</v>
-      </c>
-      <c r="F59" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="F59">
+        <v>92957</v>
       </c>
       <c r="G59" t="s">
         <v>30</v>
       </c>
       <c r="H59" s="2">
-        <v>42521</v>
+        <v>42680</v>
       </c>
       <c r="I59" s="4">
-        <v>16.489999999999998</v>
+        <v>14</v>
       </c>
       <c r="J59" t="s">
-        <v>40</v>
-      </c>
-      <c r="K59" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B60">
-        <v>2706</v>
+        <v>675097</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60">
-        <v>92912</v>
+        <v>34</v>
+      </c>
+      <c r="F60" t="s">
+        <v>39</v>
       </c>
       <c r="G60" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H60" s="2">
-        <v>42637</v>
+        <v>42521</v>
       </c>
       <c r="I60" s="4">
-        <v>13.29</v>
+        <v>16.489999999999998</v>
       </c>
       <c r="J60" t="s">
-        <v>14</v>
+        <v>40</v>
+      </c>
+      <c r="K60" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B61">
-        <v>14274</v>
+        <v>2706</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
       </c>
       <c r="F61">
-        <v>5648</v>
+        <v>92912</v>
       </c>
       <c r="G61" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H61" s="2">
-        <v>42672</v>
+        <v>42637</v>
       </c>
       <c r="I61" s="4">
-        <v>7</v>
+        <v>13.29</v>
       </c>
       <c r="J61" t="s">
-        <v>49</v>
-      </c>
-      <c r="K61" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3250,7 +3307,7 @@
         <v>47</v>
       </c>
       <c r="B62">
-        <v>14450</v>
+        <v>14274</v>
       </c>
       <c r="C62" t="s">
         <v>50</v>
@@ -3285,25 +3342,34 @@
         <v>47</v>
       </c>
       <c r="B63">
-        <v>16534</v>
+        <v>14450</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="D63" t="s">
-        <v>156</v>
+        <v>29</v>
       </c>
       <c r="E63" t="s">
-        <v>53</v>
-      </c>
-      <c r="F63" t="s">
-        <v>157</v>
+        <v>12</v>
+      </c>
+      <c r="F63">
+        <v>5648</v>
       </c>
       <c r="G63" t="s">
         <v>48</v>
       </c>
+      <c r="H63" s="2">
+        <v>42672</v>
+      </c>
+      <c r="I63" s="4">
+        <v>7</v>
+      </c>
       <c r="J63" t="s">
-        <v>158</v>
+        <v>49</v>
+      </c>
+      <c r="K63" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -3311,25 +3377,25 @@
         <v>47</v>
       </c>
       <c r="B64">
-        <v>18878</v>
+        <v>16534</v>
       </c>
       <c r="C64" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="D64" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="E64" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="F64" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G64" t="s">
         <v>48</v>
       </c>
       <c r="J64" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -3337,7 +3403,7 @@
         <v>47</v>
       </c>
       <c r="B65">
-        <v>18881</v>
+        <v>18878</v>
       </c>
       <c r="C65" t="s">
         <v>151</v>
@@ -3349,7 +3415,7 @@
         <v>97</v>
       </c>
       <c r="F65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G65" t="s">
         <v>48</v>
@@ -3363,7 +3429,7 @@
         <v>47</v>
       </c>
       <c r="B66">
-        <v>18914</v>
+        <v>18881</v>
       </c>
       <c r="C66" t="s">
         <v>151</v>
@@ -3375,7 +3441,7 @@
         <v>97</v>
       </c>
       <c r="F66" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G66" t="s">
         <v>48</v>
@@ -3389,7 +3455,7 @@
         <v>47</v>
       </c>
       <c r="B67">
-        <v>18942</v>
+        <v>18914</v>
       </c>
       <c r="C67" t="s">
         <v>151</v>
@@ -3401,7 +3467,7 @@
         <v>97</v>
       </c>
       <c r="F67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G67" t="s">
         <v>48</v>
@@ -3415,34 +3481,25 @@
         <v>47</v>
       </c>
       <c r="B68">
-        <v>20025</v>
+        <v>18942</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D68" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E68" t="s">
-        <v>139</v>
-      </c>
-      <c r="F68">
-        <v>41329</v>
+        <v>97</v>
+      </c>
+      <c r="F68" t="s">
+        <v>168</v>
       </c>
       <c r="G68" t="s">
         <v>48</v>
       </c>
-      <c r="H68" s="2">
-        <v>42608</v>
-      </c>
-      <c r="I68" s="4">
-        <v>17.989999999999998</v>
-      </c>
       <c r="J68" t="s">
-        <v>149</v>
-      </c>
-      <c r="K68" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -3450,7 +3507,7 @@
         <v>47</v>
       </c>
       <c r="B69">
-        <v>20037</v>
+        <v>20025</v>
       </c>
       <c r="C69" t="s">
         <v>138</v>
@@ -3462,7 +3519,7 @@
         <v>139</v>
       </c>
       <c r="F69">
-        <v>41330</v>
+        <v>41329</v>
       </c>
       <c r="G69" t="s">
         <v>48</v>
@@ -3485,7 +3542,7 @@
         <v>47</v>
       </c>
       <c r="B70">
-        <v>20045</v>
+        <v>20037</v>
       </c>
       <c r="C70" t="s">
         <v>138</v>
@@ -3497,7 +3554,7 @@
         <v>139</v>
       </c>
       <c r="F70">
-        <v>41331</v>
+        <v>41330</v>
       </c>
       <c r="G70" t="s">
         <v>48</v>
@@ -3520,28 +3577,34 @@
         <v>47</v>
       </c>
       <c r="B71">
-        <v>83873</v>
+        <v>20045</v>
       </c>
       <c r="C71" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E71" t="s">
-        <v>53</v>
-      </c>
-      <c r="F71" t="s">
-        <v>154</v>
+        <v>139</v>
+      </c>
+      <c r="F71">
+        <v>41331</v>
       </c>
       <c r="G71" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H71" s="2">
+        <v>42608</v>
       </c>
       <c r="I71" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J71" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K71" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -3549,7 +3612,7 @@
         <v>47</v>
       </c>
       <c r="B72">
-        <v>83916</v>
+        <v>83873</v>
       </c>
       <c r="C72" t="s">
         <v>140</v>
@@ -3561,7 +3624,7 @@
         <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G72" t="s">
         <v>55</v>
@@ -3578,7 +3641,7 @@
         <v>47</v>
       </c>
       <c r="B73">
-        <v>83950</v>
+        <v>83916</v>
       </c>
       <c r="C73" t="s">
         <v>140</v>
@@ -3590,7 +3653,7 @@
         <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G73" t="s">
         <v>55</v>
@@ -3607,7 +3670,7 @@
         <v>47</v>
       </c>
       <c r="B74">
-        <v>83987</v>
+        <v>83950</v>
       </c>
       <c r="C74" t="s">
         <v>140</v>
@@ -3619,7 +3682,7 @@
         <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G74" t="s">
         <v>55</v>
@@ -3635,26 +3698,29 @@
       <c r="A75" t="s">
         <v>47</v>
       </c>
-      <c r="B75" t="s">
-        <v>161</v>
+      <c r="B75">
+        <v>83987</v>
       </c>
       <c r="C75" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D75" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E75" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="F75" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G75" t="s">
         <v>55</v>
       </c>
+      <c r="I75" s="4">
+        <v>23.95</v>
+      </c>
       <c r="J75" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -3662,75 +3728,136 @@
         <v>47</v>
       </c>
       <c r="B76" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
       <c r="D76" t="s">
         <v>63</v>
       </c>
       <c r="E76" t="s">
-        <v>64</v>
-      </c>
-      <c r="F76">
-        <v>11347</v>
+        <v>76</v>
+      </c>
+      <c r="F76" t="s">
+        <v>163</v>
       </c>
       <c r="G76" t="s">
         <v>55</v>
       </c>
-      <c r="H76" s="2">
-        <v>42170</v>
-      </c>
-      <c r="I76" s="4">
-        <v>21.5</v>
-      </c>
       <c r="J76" t="s">
-        <v>160</v>
-      </c>
-      <c r="K76" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>206</v>
-      </c>
-      <c r="B77">
-        <v>41912</v>
+        <v>47</v>
+      </c>
+      <c r="B77" t="s">
+        <v>159</v>
       </c>
       <c r="C77" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D77" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="E77" t="s">
-        <v>207</v>
+        <v>64</v>
       </c>
       <c r="F77">
-        <v>40931302</v>
+        <v>11347</v>
       </c>
       <c r="G77" t="s">
         <v>55</v>
       </c>
       <c r="H77" s="2">
+        <v>42170</v>
+      </c>
+      <c r="I77" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J77" t="s">
+        <v>160</v>
+      </c>
+      <c r="K77" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>243</v>
+      </c>
+      <c r="B78">
+        <v>70055</v>
+      </c>
+      <c r="C78" t="s">
+        <v>134</v>
+      </c>
+      <c r="D78" t="s">
+        <v>29</v>
+      </c>
+      <c r="E78" t="s">
+        <v>34</v>
+      </c>
+      <c r="F78" t="s">
+        <v>244</v>
+      </c>
+      <c r="G78" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" s="2">
+        <v>42868</v>
+      </c>
+      <c r="I78" s="4">
+        <v>15.41</v>
+      </c>
+      <c r="J78" t="s">
+        <v>14</v>
+      </c>
+      <c r="K78" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>206</v>
+      </c>
+      <c r="B79">
+        <v>41912</v>
+      </c>
+      <c r="C79" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" t="s">
+        <v>207</v>
+      </c>
+      <c r="F79">
+        <v>40931302</v>
+      </c>
+      <c r="G79" t="s">
+        <v>55</v>
+      </c>
+      <c r="H79" s="2">
         <v>42805</v>
       </c>
-      <c r="I77" s="4">
+      <c r="I79" s="4">
         <v>9.99</v>
       </c>
-      <c r="J77" t="s">
+      <c r="J79" t="s">
         <v>208</v>
       </c>
-      <c r="K77" t="s">
+      <c r="K79" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K77">
-    <sortCondition ref="A2:A77"/>
-    <sortCondition ref="B2:B77"/>
+  <sortState ref="A2:K80">
+    <sortCondition ref="A2:A80"/>
+    <sortCondition ref="B2:B80"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3739,10 +3866,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3838,14 +3965,50 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B6" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
+        <v>74143</v>
+      </c>
       <c r="C6" t="s">
         <v>233</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="2">
+        <v>28857</v>
+      </c>
+      <c r="C8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Athearn RTR CN/GTW SD40-2
</commit_message>
<xml_diff>
--- a/trains/Inventory.xlsx
+++ b/trains/Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locomotives" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="273">
   <si>
     <t>Road Name</t>
   </si>
@@ -695,15 +695,6 @@
     <t>45477-02</t>
   </si>
   <si>
-    <t>Accurail</t>
-  </si>
-  <si>
-    <t>40' plug door boxcar</t>
-  </si>
-  <si>
-    <t>http://www.accurail.com/accurail/ART/3100/3129.jpg</t>
-  </si>
-  <si>
     <t>DT&amp;I</t>
   </si>
   <si>
@@ -725,9 +716,6 @@
     <t>20 003 806/7</t>
   </si>
   <si>
-    <t>https://kadee.com/ca/50ps1/50ps1.htm</t>
-  </si>
-  <si>
     <t>Grank Trunk</t>
   </si>
   <si>
@@ -783,6 +771,81 @@
   </si>
   <si>
     <t>train show - Pepperell</t>
+  </si>
+  <si>
+    <t>50' PS-1 cushion boxcar</t>
+  </si>
+  <si>
+    <t>train show - NVRRA</t>
+  </si>
+  <si>
+    <t>Steve's Trains</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/HO-scale-Roundhouse-RTR-Pere-Marquette-RR-36-039-old-time-box-car-train-/311922982881?hash=item48a00effe1%3Ag%3AYwYAAOSwl1hZdV5t&amp;nma=true&amp;si=yHCv4VTBDi2wFeLfV7fwAv8DYhM%253D&amp;orig_cvip=true&amp;rt=nc&amp;_trksid=p2047675.l2557</t>
+  </si>
+  <si>
+    <t>50' double-plug door boxcar</t>
+  </si>
+  <si>
+    <t>train show - NSMRC</t>
+  </si>
+  <si>
+    <t>920-101803</t>
+  </si>
+  <si>
+    <t>60' P-S single door boxcar</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/walthersproto-60-single-door-box-car-DT-I-ho-scale/332457546001?hash=item4d68039111:g:QjkAAOSw1NFaFHXm</t>
+  </si>
+  <si>
+    <t>http://www.athearn.com/Products/Default.aspx?ProdID=ATH16702</t>
+  </si>
+  <si>
+    <t>ATH16702</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>SD40-2</t>
+  </si>
+  <si>
+    <t>11354/11355</t>
+  </si>
+  <si>
+    <t>GTW/DT&amp;I</t>
+  </si>
+  <si>
+    <t>http://www.atlastrainman.com/HOFreight/tmhocupcab.htm</t>
+  </si>
+  <si>
+    <t>Stroh's box car</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/HO-scale-Athearn-Con-Cor-Strohs-Beer-DT-I-RR-50-billboard-advertising-box-car/312047229302?hash=item48a776d976:g:QgkAAOSw1RVaXqgF</t>
+  </si>
+  <si>
+    <t>Canadian National</t>
+  </si>
+  <si>
+    <t>GTW 5930</t>
+  </si>
+  <si>
+    <t>Maine Modelworks</t>
+  </si>
+  <si>
+    <t>$93.00 + $5.81 tax</t>
+  </si>
+  <si>
+    <t>N5 caboose</t>
+  </si>
+  <si>
+    <t>http://www.bowser-trains.com/new/n52017.html</t>
+  </si>
+  <si>
+    <t>41665, 41666</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,6 +1489,38 @@
         <v>180</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>16700</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="2">
+        <v>43127</v>
+      </c>
+      <c r="H8" s="4">
+        <v>98.81</v>
+      </c>
+      <c r="I8" t="s">
+        <v>268</v>
+      </c>
+      <c r="J8" t="s">
+        <v>269</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:J6">
     <sortCondition ref="A2:A6"/>
@@ -1437,11 +1532,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J82" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1624,7 +1719,7 @@
         <v>78376</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
         <v>96</v>
@@ -1648,7 +1743,7 @@
         <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2524,7 +2619,7 @@
         <v>80014</v>
       </c>
       <c r="C37" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -2545,7 +2640,7 @@
         <v>10</v>
       </c>
       <c r="J37" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2955,22 +3050,34 @@
         <v>73</v>
       </c>
       <c r="B51">
-        <v>25907</v>
+        <v>18055</v>
       </c>
       <c r="C51" t="s">
-        <v>79</v>
+        <v>248</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" t="s">
-        <v>81</v>
+        <v>207</v>
+      </c>
+      <c r="F51">
+        <v>6361</v>
       </c>
       <c r="G51" t="s">
         <v>82</v>
+      </c>
+      <c r="H51" s="2">
+        <v>43023</v>
+      </c>
+      <c r="I51" s="4">
+        <v>30</v>
+      </c>
+      <c r="J51" t="s">
+        <v>249</v>
+      </c>
+      <c r="K51" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2978,98 +3085,89 @@
         <v>73</v>
       </c>
       <c r="B52">
-        <v>32246</v>
+        <v>25907</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>24</v>
-      </c>
-      <c r="F52">
-        <v>18132</v>
+        <v>80</v>
+      </c>
+      <c r="F52" t="s">
+        <v>81</v>
       </c>
       <c r="G52" t="s">
-        <v>30</v>
-      </c>
-      <c r="H52" s="2">
-        <v>42411</v>
-      </c>
-      <c r="I52" s="4">
-        <v>12.5</v>
-      </c>
-      <c r="J52" t="s">
-        <v>90</v>
-      </c>
-      <c r="K52" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="B53">
-        <v>5546</v>
+        <v>32246</v>
       </c>
       <c r="C53" t="s">
-        <v>182</v>
+        <v>83</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
-      </c>
-      <c r="F53" t="s">
-        <v>183</v>
+        <v>24</v>
+      </c>
+      <c r="F53">
+        <v>18132</v>
       </c>
       <c r="G53" t="s">
         <v>30</v>
       </c>
       <c r="H53" s="2">
-        <v>42708</v>
+        <v>42411</v>
       </c>
       <c r="I53" s="4">
-        <v>18</v>
+        <v>12.5</v>
       </c>
       <c r="J53" t="s">
-        <v>184</v>
+        <v>90</v>
+      </c>
+      <c r="K53" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="B54">
-        <v>112115</v>
+        <v>5546</v>
       </c>
       <c r="C54" t="s">
-        <v>235</v>
+        <v>182</v>
       </c>
       <c r="D54" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E54" t="s">
         <v>64</v>
       </c>
       <c r="F54" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="G54" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H54" s="2">
-        <v>46500</v>
+        <v>42708</v>
       </c>
       <c r="I54" s="4">
-        <v>13.6</v>
+        <v>18</v>
       </c>
       <c r="J54" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -3077,10 +3175,10 @@
         <v>22</v>
       </c>
       <c r="B55">
-        <v>112143</v>
+        <v>112115</v>
       </c>
       <c r="C55" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D55" t="s">
         <v>29</v>
@@ -3089,22 +3187,19 @@
         <v>64</v>
       </c>
       <c r="F55" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G55" t="s">
         <v>19</v>
       </c>
       <c r="H55" s="2">
-        <v>42793</v>
+        <v>46500</v>
       </c>
       <c r="I55" s="4">
-        <v>18</v>
+        <v>13.6</v>
       </c>
       <c r="J55" t="s">
-        <v>238</v>
-      </c>
-      <c r="K55" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -3112,34 +3207,34 @@
         <v>22</v>
       </c>
       <c r="B56">
-        <v>113894</v>
+        <v>112143</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>231</v>
       </c>
       <c r="D56" t="s">
         <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56">
-        <v>93725</v>
+        <v>64</v>
+      </c>
+      <c r="F56" t="s">
+        <v>236</v>
       </c>
       <c r="G56" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H56" s="2">
-        <v>42709</v>
+        <v>42793</v>
       </c>
       <c r="I56" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="J56" t="s">
-        <v>32</v>
+        <v>234</v>
       </c>
       <c r="K56" t="s">
-        <v>31</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -3147,25 +3242,34 @@
         <v>22</v>
       </c>
       <c r="B57">
-        <v>148077</v>
+        <v>113894</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D57" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="F57">
+        <v>93725</v>
       </c>
       <c r="G57" t="s">
         <v>30</v>
       </c>
+      <c r="H57" s="2">
+        <v>42709</v>
+      </c>
       <c r="I57" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J57" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="K57" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -3173,34 +3277,25 @@
         <v>22</v>
       </c>
       <c r="B58">
-        <v>591263</v>
+        <v>148077</v>
       </c>
       <c r="C58" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E58" t="s">
-        <v>34</v>
-      </c>
-      <c r="F58" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G58" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="2">
-        <v>42440</v>
+        <v>30</v>
       </c>
       <c r="I58" s="4">
-        <v>14.99</v>
+        <v>12</v>
       </c>
       <c r="J58" t="s">
-        <v>36</v>
-      </c>
-      <c r="K58" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -3208,10 +3303,10 @@
         <v>22</v>
       </c>
       <c r="B59">
-        <v>598016</v>
+        <v>302157</v>
       </c>
       <c r="C59" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -3220,19 +3315,22 @@
         <v>12</v>
       </c>
       <c r="F59">
-        <v>92957</v>
+        <v>91356</v>
       </c>
       <c r="G59" t="s">
         <v>30</v>
       </c>
       <c r="H59" s="2">
-        <v>42680</v>
+        <v>43029</v>
       </c>
       <c r="I59" s="4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J59" t="s">
-        <v>58</v>
+        <v>253</v>
+      </c>
+      <c r="K59" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -3240,45 +3338,45 @@
         <v>22</v>
       </c>
       <c r="B60">
-        <v>675097</v>
+        <v>591263</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
       </c>
       <c r="F60" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G60" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H60" s="2">
-        <v>42521</v>
+        <v>42440</v>
       </c>
       <c r="I60" s="4">
-        <v>16.489999999999998</v>
+        <v>14.99</v>
       </c>
       <c r="J60" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B61">
-        <v>2706</v>
+        <v>598016</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>230</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -3287,89 +3385,86 @@
         <v>12</v>
       </c>
       <c r="F61">
-        <v>92912</v>
+        <v>92957</v>
       </c>
       <c r="G61" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H61" s="2">
-        <v>42637</v>
+        <v>42680</v>
       </c>
       <c r="I61" s="4">
-        <v>13.29</v>
+        <v>14</v>
       </c>
       <c r="J61" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B62">
-        <v>14274</v>
+        <v>675097</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E62" t="s">
-        <v>12</v>
-      </c>
-      <c r="F62">
-        <v>5648</v>
+        <v>34</v>
+      </c>
+      <c r="F62" t="s">
+        <v>39</v>
       </c>
       <c r="G62" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H62" s="2">
-        <v>42672</v>
+        <v>42521</v>
       </c>
       <c r="I62" s="4">
-        <v>7</v>
+        <v>16.489999999999998</v>
       </c>
       <c r="J62" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K62" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B63">
-        <v>14450</v>
+        <v>2706</v>
       </c>
       <c r="C63" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E63" t="s">
         <v>12</v>
       </c>
       <c r="F63">
-        <v>5648</v>
+        <v>92912</v>
       </c>
       <c r="G63" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H63" s="2">
-        <v>42672</v>
+        <v>42637</v>
       </c>
       <c r="I63" s="4">
-        <v>7</v>
+        <v>13.29</v>
       </c>
       <c r="J63" t="s">
-        <v>49</v>
-      </c>
-      <c r="K63" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -3377,25 +3472,34 @@
         <v>47</v>
       </c>
       <c r="B64">
-        <v>16534</v>
+        <v>14274</v>
       </c>
       <c r="C64" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="D64" t="s">
-        <v>156</v>
+        <v>29</v>
       </c>
       <c r="E64" t="s">
-        <v>53</v>
-      </c>
-      <c r="F64" t="s">
-        <v>157</v>
+        <v>12</v>
+      </c>
+      <c r="F64">
+        <v>5648</v>
       </c>
       <c r="G64" t="s">
         <v>48</v>
       </c>
+      <c r="H64" s="2">
+        <v>42672</v>
+      </c>
+      <c r="I64" s="4">
+        <v>7</v>
+      </c>
       <c r="J64" t="s">
-        <v>158</v>
+        <v>49</v>
+      </c>
+      <c r="K64" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -3403,25 +3507,34 @@
         <v>47</v>
       </c>
       <c r="B65">
-        <v>18878</v>
+        <v>14450</v>
       </c>
       <c r="C65" t="s">
-        <v>151</v>
+        <v>50</v>
       </c>
       <c r="D65" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F65" t="s">
-        <v>165</v>
+        <v>12</v>
+      </c>
+      <c r="F65">
+        <v>5648</v>
       </c>
       <c r="G65" t="s">
         <v>48</v>
       </c>
+      <c r="H65" s="2">
+        <v>42672</v>
+      </c>
+      <c r="I65" s="4">
+        <v>7</v>
+      </c>
       <c r="J65" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="K65" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -3429,25 +3542,25 @@
         <v>47</v>
       </c>
       <c r="B66">
-        <v>18881</v>
+        <v>16534</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="D66" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="E66" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="G66" t="s">
         <v>48</v>
       </c>
       <c r="J66" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -3455,7 +3568,7 @@
         <v>47</v>
       </c>
       <c r="B67">
-        <v>18914</v>
+        <v>18878</v>
       </c>
       <c r="C67" t="s">
         <v>151</v>
@@ -3467,7 +3580,7 @@
         <v>97</v>
       </c>
       <c r="F67" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G67" t="s">
         <v>48</v>
@@ -3481,7 +3594,7 @@
         <v>47</v>
       </c>
       <c r="B68">
-        <v>18942</v>
+        <v>18881</v>
       </c>
       <c r="C68" t="s">
         <v>151</v>
@@ -3493,7 +3606,7 @@
         <v>97</v>
       </c>
       <c r="F68" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G68" t="s">
         <v>48</v>
@@ -3507,34 +3620,25 @@
         <v>47</v>
       </c>
       <c r="B69">
-        <v>20025</v>
+        <v>18914</v>
       </c>
       <c r="C69" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E69" t="s">
-        <v>139</v>
-      </c>
-      <c r="F69">
-        <v>41329</v>
+        <v>97</v>
+      </c>
+      <c r="F69" t="s">
+        <v>167</v>
       </c>
       <c r="G69" t="s">
         <v>48</v>
       </c>
-      <c r="H69" s="2">
-        <v>42608</v>
-      </c>
-      <c r="I69" s="4">
-        <v>17.989999999999998</v>
-      </c>
       <c r="J69" t="s">
-        <v>149</v>
-      </c>
-      <c r="K69" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -3542,34 +3646,25 @@
         <v>47</v>
       </c>
       <c r="B70">
-        <v>20037</v>
+        <v>18942</v>
       </c>
       <c r="C70" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D70" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E70" t="s">
-        <v>139</v>
-      </c>
-      <c r="F70">
-        <v>41330</v>
+        <v>97</v>
+      </c>
+      <c r="F70" t="s">
+        <v>168</v>
       </c>
       <c r="G70" t="s">
         <v>48</v>
       </c>
-      <c r="H70" s="2">
-        <v>42608</v>
-      </c>
-      <c r="I70" s="4">
-        <v>17.989999999999998</v>
-      </c>
       <c r="J70" t="s">
-        <v>149</v>
-      </c>
-      <c r="K70" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -3577,7 +3672,7 @@
         <v>47</v>
       </c>
       <c r="B71">
-        <v>20045</v>
+        <v>20025</v>
       </c>
       <c r="C71" t="s">
         <v>138</v>
@@ -3589,7 +3684,7 @@
         <v>139</v>
       </c>
       <c r="F71">
-        <v>41331</v>
+        <v>41329</v>
       </c>
       <c r="G71" t="s">
         <v>48</v>
@@ -3612,28 +3707,34 @@
         <v>47</v>
       </c>
       <c r="B72">
-        <v>83873</v>
+        <v>20037</v>
       </c>
       <c r="C72" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D72" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E72" t="s">
-        <v>53</v>
-      </c>
-      <c r="F72" t="s">
-        <v>154</v>
+        <v>139</v>
+      </c>
+      <c r="F72">
+        <v>41330</v>
       </c>
       <c r="G72" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H72" s="2">
+        <v>42608</v>
       </c>
       <c r="I72" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J72" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K72" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -3641,28 +3742,34 @@
         <v>47</v>
       </c>
       <c r="B73">
-        <v>83916</v>
+        <v>20045</v>
       </c>
       <c r="C73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E73" t="s">
-        <v>53</v>
-      </c>
-      <c r="F73" t="s">
-        <v>155</v>
+        <v>139</v>
+      </c>
+      <c r="F73">
+        <v>41331</v>
       </c>
       <c r="G73" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H73" s="2">
+        <v>42608</v>
       </c>
       <c r="I73" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J73" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K73" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -3670,7 +3777,7 @@
         <v>47</v>
       </c>
       <c r="B74">
-        <v>83950</v>
+        <v>83873</v>
       </c>
       <c r="C74" t="s">
         <v>140</v>
@@ -3682,7 +3789,7 @@
         <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G74" t="s">
         <v>55</v>
@@ -3699,7 +3806,7 @@
         <v>47</v>
       </c>
       <c r="B75">
-        <v>83987</v>
+        <v>83916</v>
       </c>
       <c r="C75" t="s">
         <v>140</v>
@@ -3711,7 +3818,7 @@
         <v>53</v>
       </c>
       <c r="F75" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G75" t="s">
         <v>55</v>
@@ -3727,137 +3834,195 @@
       <c r="A76" t="s">
         <v>47</v>
       </c>
-      <c r="B76" t="s">
-        <v>161</v>
+      <c r="B76">
+        <v>83950</v>
       </c>
       <c r="C76" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D76" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E76" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="G76" t="s">
         <v>55</v>
       </c>
+      <c r="I76" s="4">
+        <v>23.95</v>
+      </c>
       <c r="J76" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>47</v>
       </c>
-      <c r="B77" t="s">
-        <v>159</v>
+      <c r="B77">
+        <v>83987</v>
       </c>
       <c r="C77" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="D77" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E77" t="s">
-        <v>64</v>
-      </c>
-      <c r="F77">
-        <v>11347</v>
+        <v>53</v>
+      </c>
+      <c r="F77" t="s">
+        <v>153</v>
       </c>
       <c r="G77" t="s">
         <v>55</v>
       </c>
-      <c r="H77" s="2">
-        <v>42170</v>
-      </c>
       <c r="I77" s="4">
-        <v>21.5</v>
+        <v>23.95</v>
       </c>
       <c r="J77" t="s">
-        <v>160</v>
-      </c>
-      <c r="K77" t="s">
-        <v>164</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>243</v>
-      </c>
-      <c r="B78">
-        <v>70055</v>
+        <v>47</v>
+      </c>
+      <c r="B78" t="s">
+        <v>161</v>
       </c>
       <c r="C78" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="D78" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E78" t="s">
+        <v>76</v>
+      </c>
+      <c r="F78" t="s">
+        <v>163</v>
+      </c>
+      <c r="G78" t="s">
+        <v>55</v>
+      </c>
+      <c r="J78" t="s">
         <v>34</v>
-      </c>
-      <c r="F78" t="s">
-        <v>244</v>
-      </c>
-      <c r="G78" t="s">
-        <v>19</v>
-      </c>
-      <c r="H78" s="2">
-        <v>42868</v>
-      </c>
-      <c r="I78" s="4">
-        <v>15.41</v>
-      </c>
-      <c r="J78" t="s">
-        <v>14</v>
-      </c>
-      <c r="K78" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>206</v>
-      </c>
-      <c r="B79">
-        <v>41912</v>
+        <v>47</v>
+      </c>
+      <c r="B79" t="s">
+        <v>159</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="E79" t="s">
-        <v>207</v>
+        <v>64</v>
       </c>
       <c r="F79">
-        <v>40931302</v>
+        <v>11347</v>
       </c>
       <c r="G79" t="s">
         <v>55</v>
       </c>
       <c r="H79" s="2">
+        <v>42170</v>
+      </c>
+      <c r="I79" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J79" t="s">
+        <v>160</v>
+      </c>
+      <c r="K79" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>239</v>
+      </c>
+      <c r="B80">
+        <v>70055</v>
+      </c>
+      <c r="C80" t="s">
+        <v>134</v>
+      </c>
+      <c r="D80" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" t="s">
+        <v>34</v>
+      </c>
+      <c r="F80" t="s">
+        <v>240</v>
+      </c>
+      <c r="G80" t="s">
+        <v>19</v>
+      </c>
+      <c r="H80" s="2">
+        <v>42868</v>
+      </c>
+      <c r="I80" s="4">
+        <v>15.41</v>
+      </c>
+      <c r="J80" t="s">
+        <v>14</v>
+      </c>
+      <c r="K80" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>206</v>
+      </c>
+      <c r="B81">
+        <v>41912</v>
+      </c>
+      <c r="C81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" t="s">
+        <v>207</v>
+      </c>
+      <c r="F81">
+        <v>40931302</v>
+      </c>
+      <c r="G81" t="s">
+        <v>55</v>
+      </c>
+      <c r="H81" s="2">
         <v>42805</v>
       </c>
-      <c r="I79" s="4">
+      <c r="I81" s="4">
         <v>9.99</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J81" t="s">
         <v>208</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K81" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K80">
-    <sortCondition ref="A2:A80"/>
-    <sortCondition ref="B2:B80"/>
+  <sortState ref="A2:K81">
+    <sortCondition ref="A2:A81"/>
+    <sortCondition ref="B2:B81"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3866,10 +4031,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3903,112 +4068,174 @@
         <v>97324</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3">
-        <v>3129</v>
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
       </c>
       <c r="C3" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>231</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="9">
+        <v>74143</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5">
-        <v>6361</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="9">
-        <v>74143</v>
+        <v>64</v>
+      </c>
+      <c r="B6" s="2">
+        <v>28857</v>
       </c>
       <c r="C6" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>246</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="2">
-        <v>28857</v>
-      </c>
-      <c r="C8" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>249</v>
+      <c r="B10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>270</v>
+      </c>
+      <c r="E12" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Michigan Central, Pere Marquette box cars
</commit_message>
<xml_diff>
--- a/trains/Inventory.xlsx
+++ b/trains/Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Locomotives" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="279">
   <si>
     <t>Road Name</t>
   </si>
@@ -812,15 +812,6 @@
     <t>SD40-2</t>
   </si>
   <si>
-    <t>11354/11355</t>
-  </si>
-  <si>
-    <t>GTW/DT&amp;I</t>
-  </si>
-  <si>
-    <t>http://www.atlastrainman.com/HOFreight/tmhocupcab.htm</t>
-  </si>
-  <si>
     <t>Stroh's box car</t>
   </si>
   <si>
@@ -846,6 +837,33 @@
   </si>
   <si>
     <t>41665, 41666</t>
+  </si>
+  <si>
+    <t>eBay - wuggy141</t>
+  </si>
+  <si>
+    <t>$7.10 shipping</t>
+  </si>
+  <si>
+    <t>2-8-4 Berkshire</t>
+  </si>
+  <si>
+    <t>Silver City Hobby</t>
+  </si>
+  <si>
+    <t>Alco S2</t>
+  </si>
+  <si>
+    <t>10 001 484</t>
+  </si>
+  <si>
+    <t>40' Youngstown boxcar</t>
+  </si>
+  <si>
+    <t>$1.22 tax, 30% off sale</t>
+  </si>
+  <si>
+    <t>eBay - mrisfun</t>
   </si>
 </sst>
 </file>
@@ -923,7 +941,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -932,6 +949,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1270,15 +1288,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
     <col min="8" max="8" width="10.83203125" style="4"/>
     <col min="9" max="9" width="21.83203125" customWidth="1"/>
   </cols>
@@ -1302,7 +1321,7 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1320,22 +1339,22 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>1360</v>
+        <v>1260</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>274</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2">
-        <v>51811</v>
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>275</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
       </c>
       <c r="H2" s="4">
-        <v>119.95</v>
+        <v>152.94999999999999</v>
       </c>
       <c r="I2" t="s">
         <v>68</v>
@@ -1346,22 +1365,22 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>1536</v>
+        <v>1360</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
       </c>
       <c r="E3">
-        <v>63903</v>
+        <v>51811</v>
       </c>
       <c r="F3" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="H3" s="4">
-        <v>114.95</v>
+        <v>119.95</v>
       </c>
       <c r="I3" t="s">
         <v>68</v>
@@ -1369,162 +1388,217 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>281</v>
+        <v>1536</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="E4">
-        <v>9388</v>
+        <v>63903</v>
       </c>
       <c r="F4" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4" s="5">
-        <v>42479</v>
+        <v>148</v>
       </c>
       <c r="H4" s="4">
-        <v>109</v>
+        <v>114.95</v>
       </c>
       <c r="I4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J4" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>405</v>
+        <v>1575</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5">
-        <v>66304</v>
+        <v>65605</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="H5" s="4">
-        <v>114.99</v>
+        <v>112.95</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>8087</v>
+        <v>263</v>
+      </c>
+      <c r="B6" t="s">
+        <v>264</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>260</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>63211</v>
+        <v>16700</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G6" s="2">
-        <v>42429</v>
+        <v>43127</v>
       </c>
       <c r="H6" s="4">
-        <v>99.99</v>
+        <v>98.81</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B7">
-        <v>1575</v>
+        <v>281</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E7">
-        <v>65605</v>
+        <v>9388</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>120</v>
+      </c>
+      <c r="G7" s="2">
+        <v>42479</v>
       </c>
       <c r="H7" s="4">
-        <v>112.95</v>
+        <v>109</v>
       </c>
       <c r="I7" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="J7" t="s">
-        <v>180</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>266</v>
-      </c>
-      <c r="B8" t="s">
-        <v>267</v>
+        <v>69</v>
+      </c>
+      <c r="B8">
+        <v>405</v>
       </c>
       <c r="C8" t="s">
-        <v>260</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E8">
-        <v>16700</v>
+        <v>66304</v>
       </c>
       <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="4">
+        <v>114.99</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>8087</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>63211</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2">
+        <v>42429</v>
+      </c>
+      <c r="H9" s="4">
+        <v>99.99</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>1225</v>
+      </c>
+      <c r="C10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>52403</v>
+      </c>
+      <c r="F10" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="2">
-        <v>43127</v>
-      </c>
-      <c r="H8" s="4">
-        <v>98.81</v>
-      </c>
-      <c r="I8" t="s">
-        <v>268</v>
-      </c>
-      <c r="J8" t="s">
-        <v>269</v>
+      <c r="G10" s="2">
+        <v>41981</v>
+      </c>
+      <c r="H10" s="4">
+        <v>188.95</v>
+      </c>
+      <c r="I10" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J6">
-    <sortCondition ref="A2:A6"/>
-    <sortCondition ref="B2:B6"/>
+  <sortState ref="A2:J10">
+    <sortCondition ref="A2:A10"/>
+    <sortCondition ref="B2:B10"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1532,11 +1606,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J82" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2290,7 +2364,7 @@
       <c r="G26" t="s">
         <v>48</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="7">
         <v>42785</v>
       </c>
       <c r="I26" s="4">
@@ -3175,31 +3249,34 @@
         <v>22</v>
       </c>
       <c r="B55">
-        <v>112115</v>
+        <v>153</v>
       </c>
       <c r="C55" t="s">
-        <v>231</v>
+        <v>62</v>
       </c>
       <c r="D55" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E55" t="s">
         <v>64</v>
       </c>
-      <c r="F55" t="s">
-        <v>232</v>
+      <c r="F55">
+        <v>11355</v>
       </c>
       <c r="G55" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H55" s="2">
-        <v>46500</v>
+        <v>43150</v>
       </c>
       <c r="I55" s="4">
-        <v>13.6</v>
+        <v>15.27</v>
       </c>
       <c r="J55" t="s">
-        <v>233</v>
+        <v>270</v>
+      </c>
+      <c r="K55" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -3207,7 +3284,7 @@
         <v>22</v>
       </c>
       <c r="B56">
-        <v>112143</v>
+        <v>112115</v>
       </c>
       <c r="C56" t="s">
         <v>231</v>
@@ -3219,22 +3296,19 @@
         <v>64</v>
       </c>
       <c r="F56" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G56" t="s">
         <v>19</v>
       </c>
       <c r="H56" s="2">
-        <v>42793</v>
+        <v>46500</v>
       </c>
       <c r="I56" s="4">
-        <v>18</v>
+        <v>13.6</v>
       </c>
       <c r="J56" t="s">
-        <v>234</v>
-      </c>
-      <c r="K56" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -3242,34 +3316,34 @@
         <v>22</v>
       </c>
       <c r="B57">
-        <v>113894</v>
+        <v>112143</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>231</v>
       </c>
       <c r="D57" t="s">
         <v>29</v>
       </c>
       <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57">
-        <v>93725</v>
+        <v>64</v>
+      </c>
+      <c r="F57" t="s">
+        <v>236</v>
       </c>
       <c r="G57" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H57" s="2">
-        <v>42709</v>
+        <v>42793</v>
       </c>
       <c r="I57" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="J57" t="s">
-        <v>32</v>
+        <v>234</v>
       </c>
       <c r="K57" t="s">
-        <v>31</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -3277,25 +3351,34 @@
         <v>22</v>
       </c>
       <c r="B58">
-        <v>148077</v>
+        <v>113894</v>
       </c>
       <c r="C58" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D58" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E58" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="F58">
+        <v>93725</v>
       </c>
       <c r="G58" t="s">
         <v>30</v>
       </c>
+      <c r="H58" s="2">
+        <v>42709</v>
+      </c>
       <c r="I58" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J58" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="K58" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -3303,34 +3386,25 @@
         <v>22</v>
       </c>
       <c r="B59">
-        <v>302157</v>
+        <v>148077</v>
       </c>
       <c r="C59" t="s">
-        <v>252</v>
+        <v>46</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59">
-        <v>91356</v>
+        <v>44</v>
       </c>
       <c r="G59" t="s">
         <v>30</v>
       </c>
-      <c r="H59" s="2">
-        <v>43029</v>
-      </c>
       <c r="I59" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J59" t="s">
-        <v>253</v>
-      </c>
-      <c r="K59" t="s">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -3338,34 +3412,34 @@
         <v>22</v>
       </c>
       <c r="B60">
-        <v>591263</v>
+        <v>302157</v>
       </c>
       <c r="C60" t="s">
-        <v>33</v>
+        <v>252</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
       </c>
       <c r="E60" t="s">
-        <v>34</v>
-      </c>
-      <c r="F60" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="F60">
+        <v>91356</v>
       </c>
       <c r="G60" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H60" s="2">
-        <v>42440</v>
+        <v>43029</v>
       </c>
       <c r="I60" s="4">
-        <v>14.99</v>
+        <v>10</v>
       </c>
       <c r="J60" t="s">
-        <v>36</v>
+        <v>253</v>
       </c>
       <c r="K60" t="s">
-        <v>42</v>
+        <v>250</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -3373,31 +3447,34 @@
         <v>22</v>
       </c>
       <c r="B61">
-        <v>598016</v>
+        <v>591263</v>
       </c>
       <c r="C61" t="s">
-        <v>230</v>
+        <v>33</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61">
-        <v>92957</v>
+        <v>34</v>
+      </c>
+      <c r="F61" t="s">
+        <v>35</v>
       </c>
       <c r="G61" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H61" s="2">
-        <v>42680</v>
+        <v>42440</v>
       </c>
       <c r="I61" s="4">
-        <v>14</v>
+        <v>14.99</v>
       </c>
       <c r="J61" t="s">
-        <v>58</v>
+        <v>36</v>
+      </c>
+      <c r="K61" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3405,136 +3482,133 @@
         <v>22</v>
       </c>
       <c r="B62">
-        <v>675097</v>
+        <v>598016</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>230</v>
       </c>
       <c r="D62" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E62" t="s">
-        <v>34</v>
-      </c>
-      <c r="F62" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="F62">
+        <v>92957</v>
       </c>
       <c r="G62" t="s">
         <v>30</v>
       </c>
       <c r="H62" s="2">
-        <v>42521</v>
+        <v>42680</v>
       </c>
       <c r="I62" s="4">
-        <v>16.489999999999998</v>
+        <v>14</v>
       </c>
       <c r="J62" t="s">
-        <v>40</v>
-      </c>
-      <c r="K62" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B63">
-        <v>2706</v>
+        <v>675097</v>
       </c>
       <c r="C63" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E63" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63">
-        <v>92912</v>
+        <v>34</v>
+      </c>
+      <c r="F63" t="s">
+        <v>39</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H63" s="2">
-        <v>42637</v>
+        <v>42521</v>
       </c>
       <c r="I63" s="4">
-        <v>13.29</v>
+        <v>16.489999999999998</v>
       </c>
       <c r="J63" t="s">
-        <v>14</v>
+        <v>40</v>
+      </c>
+      <c r="K63" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B64">
-        <v>14274</v>
+        <v>2706</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D64" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
       </c>
       <c r="F64">
-        <v>5648</v>
+        <v>92912</v>
       </c>
       <c r="G64" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H64" s="2">
-        <v>42672</v>
+        <v>42637</v>
       </c>
       <c r="I64" s="4">
-        <v>7</v>
+        <v>13.29</v>
       </c>
       <c r="J64" t="s">
-        <v>49</v>
-      </c>
-      <c r="K64" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
       <c r="B65">
-        <v>14450</v>
+        <v>80948</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>276</v>
       </c>
       <c r="D65" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
       </c>
       <c r="F65">
-        <v>5648</v>
+        <v>73518</v>
       </c>
       <c r="G65" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H65" s="2">
-        <v>42672</v>
+        <v>43248</v>
       </c>
       <c r="I65" s="4">
-        <v>7</v>
+        <v>19.59</v>
       </c>
       <c r="J65" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="K65" t="s">
-        <v>66</v>
+        <v>277</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -3542,25 +3616,34 @@
         <v>47</v>
       </c>
       <c r="B66">
-        <v>16534</v>
+        <v>14274</v>
       </c>
       <c r="C66" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="D66" t="s">
-        <v>156</v>
+        <v>29</v>
       </c>
       <c r="E66" t="s">
-        <v>53</v>
-      </c>
-      <c r="F66" t="s">
-        <v>157</v>
+        <v>12</v>
+      </c>
+      <c r="F66">
+        <v>5648</v>
       </c>
       <c r="G66" t="s">
         <v>48</v>
       </c>
+      <c r="H66" s="2">
+        <v>42672</v>
+      </c>
+      <c r="I66" s="4">
+        <v>7</v>
+      </c>
       <c r="J66" t="s">
-        <v>158</v>
+        <v>49</v>
+      </c>
+      <c r="K66" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -3568,25 +3651,34 @@
         <v>47</v>
       </c>
       <c r="B67">
-        <v>18878</v>
+        <v>14450</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>50</v>
       </c>
       <c r="D67" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E67" t="s">
-        <v>97</v>
-      </c>
-      <c r="F67" t="s">
-        <v>165</v>
+        <v>12</v>
+      </c>
+      <c r="F67">
+        <v>5648</v>
       </c>
       <c r="G67" t="s">
         <v>48</v>
       </c>
+      <c r="H67" s="2">
+        <v>42672</v>
+      </c>
+      <c r="I67" s="4">
+        <v>7</v>
+      </c>
       <c r="J67" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="K67" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -3594,25 +3686,25 @@
         <v>47</v>
       </c>
       <c r="B68">
-        <v>18881</v>
+        <v>16534</v>
       </c>
       <c r="C68" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="D68" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="E68" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="F68" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="G68" t="s">
         <v>48</v>
       </c>
       <c r="J68" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -3620,7 +3712,7 @@
         <v>47</v>
       </c>
       <c r="B69">
-        <v>18914</v>
+        <v>18878</v>
       </c>
       <c r="C69" t="s">
         <v>151</v>
@@ -3632,13 +3724,19 @@
         <v>97</v>
       </c>
       <c r="F69" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G69" t="s">
         <v>48</v>
       </c>
+      <c r="I69" s="4">
+        <v>10</v>
+      </c>
       <c r="J69" t="s">
         <v>45</v>
+      </c>
+      <c r="K69" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -3646,7 +3744,7 @@
         <v>47</v>
       </c>
       <c r="B70">
-        <v>18942</v>
+        <v>18881</v>
       </c>
       <c r="C70" t="s">
         <v>151</v>
@@ -3658,13 +3756,19 @@
         <v>97</v>
       </c>
       <c r="F70" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G70" t="s">
         <v>48</v>
       </c>
+      <c r="I70" s="4">
+        <v>10</v>
+      </c>
       <c r="J70" t="s">
         <v>45</v>
+      </c>
+      <c r="K70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -3672,34 +3776,31 @@
         <v>47</v>
       </c>
       <c r="B71">
-        <v>20025</v>
+        <v>18914</v>
       </c>
       <c r="C71" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D71" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E71" t="s">
-        <v>139</v>
-      </c>
-      <c r="F71">
-        <v>41329</v>
+        <v>97</v>
+      </c>
+      <c r="F71" t="s">
+        <v>167</v>
       </c>
       <c r="G71" t="s">
         <v>48</v>
       </c>
-      <c r="H71" s="2">
-        <v>42608</v>
-      </c>
       <c r="I71" s="4">
-        <v>17.989999999999998</v>
+        <v>10</v>
       </c>
       <c r="J71" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="K71" t="s">
-        <v>150</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -3707,34 +3808,31 @@
         <v>47</v>
       </c>
       <c r="B72">
-        <v>20037</v>
+        <v>18942</v>
       </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D72" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E72" t="s">
-        <v>139</v>
-      </c>
-      <c r="F72">
-        <v>41330</v>
+        <v>97</v>
+      </c>
+      <c r="F72" t="s">
+        <v>168</v>
       </c>
       <c r="G72" t="s">
         <v>48</v>
       </c>
-      <c r="H72" s="2">
-        <v>42608</v>
-      </c>
       <c r="I72" s="4">
-        <v>17.989999999999998</v>
+        <v>10</v>
       </c>
       <c r="J72" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="K72" t="s">
-        <v>150</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -3742,7 +3840,7 @@
         <v>47</v>
       </c>
       <c r="B73">
-        <v>20045</v>
+        <v>20025</v>
       </c>
       <c r="C73" t="s">
         <v>138</v>
@@ -3754,7 +3852,7 @@
         <v>139</v>
       </c>
       <c r="F73">
-        <v>41331</v>
+        <v>41329</v>
       </c>
       <c r="G73" t="s">
         <v>48</v>
@@ -3777,28 +3875,34 @@
         <v>47</v>
       </c>
       <c r="B74">
-        <v>83873</v>
+        <v>20037</v>
       </c>
       <c r="C74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E74" t="s">
-        <v>53</v>
-      </c>
-      <c r="F74" t="s">
-        <v>154</v>
+        <v>139</v>
+      </c>
+      <c r="F74">
+        <v>41330</v>
       </c>
       <c r="G74" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H74" s="2">
+        <v>42608</v>
       </c>
       <c r="I74" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J74" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K74" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -3806,28 +3910,34 @@
         <v>47</v>
       </c>
       <c r="B75">
-        <v>83916</v>
+        <v>20045</v>
       </c>
       <c r="C75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E75" t="s">
-        <v>53</v>
-      </c>
-      <c r="F75" t="s">
-        <v>155</v>
+        <v>139</v>
+      </c>
+      <c r="F75">
+        <v>41331</v>
       </c>
       <c r="G75" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H75" s="2">
+        <v>42608</v>
       </c>
       <c r="I75" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J75" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K75" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -3835,28 +3945,34 @@
         <v>47</v>
       </c>
       <c r="B76">
-        <v>83950</v>
+        <v>30196</v>
       </c>
       <c r="C76" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
       </c>
       <c r="E76" t="s">
-        <v>53</v>
-      </c>
-      <c r="F76" t="s">
-        <v>152</v>
+        <v>171</v>
+      </c>
+      <c r="F76">
+        <v>84189</v>
       </c>
       <c r="G76" t="s">
         <v>55</v>
       </c>
+      <c r="H76" s="2">
+        <v>43232</v>
+      </c>
       <c r="I76" s="4">
-        <v>23.95</v>
+        <v>34.56</v>
       </c>
       <c r="J76" t="s">
-        <v>68</v>
+        <v>278</v>
+      </c>
+      <c r="K76" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3864,7 +3980,7 @@
         <v>47</v>
       </c>
       <c r="B77">
-        <v>83987</v>
+        <v>83873</v>
       </c>
       <c r="C77" t="s">
         <v>140</v>
@@ -3876,7 +3992,7 @@
         <v>53</v>
       </c>
       <c r="F77" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G77" t="s">
         <v>55</v>
@@ -3892,137 +4008,224 @@
       <c r="A78" t="s">
         <v>47</v>
       </c>
-      <c r="B78" t="s">
-        <v>161</v>
+      <c r="B78">
+        <v>83916</v>
       </c>
       <c r="C78" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D78" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E78" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="F78" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="G78" t="s">
         <v>55</v>
       </c>
+      <c r="I78" s="4">
+        <v>23.95</v>
+      </c>
       <c r="J78" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>47</v>
       </c>
-      <c r="B79" t="s">
-        <v>159</v>
+      <c r="B79">
+        <v>83950</v>
       </c>
       <c r="C79" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="D79" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E79" t="s">
-        <v>64</v>
-      </c>
-      <c r="F79">
-        <v>11347</v>
+        <v>53</v>
+      </c>
+      <c r="F79" t="s">
+        <v>152</v>
       </c>
       <c r="G79" t="s">
         <v>55</v>
       </c>
-      <c r="H79" s="2">
-        <v>42170</v>
-      </c>
       <c r="I79" s="4">
-        <v>21.5</v>
+        <v>23.95</v>
       </c>
       <c r="J79" t="s">
-        <v>160</v>
-      </c>
-      <c r="K79" t="s">
-        <v>164</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>239</v>
+        <v>47</v>
       </c>
       <c r="B80">
-        <v>70055</v>
+        <v>83987</v>
       </c>
       <c r="C80" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D80" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E80" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F80" t="s">
-        <v>240</v>
+        <v>153</v>
       </c>
       <c r="G80" t="s">
-        <v>19</v>
-      </c>
-      <c r="H80" s="2">
-        <v>42868</v>
+        <v>55</v>
       </c>
       <c r="I80" s="4">
-        <v>15.41</v>
+        <v>23.95</v>
       </c>
       <c r="J80" t="s">
-        <v>14</v>
-      </c>
-      <c r="K80" t="s">
-        <v>241</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>206</v>
-      </c>
-      <c r="B81">
-        <v>41912</v>
+        <v>47</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="E81" t="s">
-        <v>207</v>
-      </c>
-      <c r="F81">
-        <v>40931302</v>
+        <v>76</v>
+      </c>
+      <c r="F81" t="s">
+        <v>163</v>
       </c>
       <c r="G81" t="s">
         <v>55</v>
       </c>
-      <c r="H81" s="2">
+      <c r="J81" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>47</v>
+      </c>
+      <c r="B82" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D82" t="s">
+        <v>63</v>
+      </c>
+      <c r="E82" t="s">
+        <v>64</v>
+      </c>
+      <c r="F82">
+        <v>11347</v>
+      </c>
+      <c r="G82" t="s">
+        <v>55</v>
+      </c>
+      <c r="H82" s="2">
+        <v>42170</v>
+      </c>
+      <c r="I82" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J82" t="s">
+        <v>160</v>
+      </c>
+      <c r="K82" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>239</v>
+      </c>
+      <c r="B83">
+        <v>70055</v>
+      </c>
+      <c r="C83" t="s">
+        <v>134</v>
+      </c>
+      <c r="D83" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" t="s">
+        <v>34</v>
+      </c>
+      <c r="F83" t="s">
+        <v>240</v>
+      </c>
+      <c r="G83" t="s">
+        <v>19</v>
+      </c>
+      <c r="H83" s="2">
+        <v>42868</v>
+      </c>
+      <c r="I83" s="4">
+        <v>15.41</v>
+      </c>
+      <c r="J83" t="s">
+        <v>14</v>
+      </c>
+      <c r="K83" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84">
+        <v>41912</v>
+      </c>
+      <c r="C84" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
+        <v>207</v>
+      </c>
+      <c r="F84">
+        <v>40931302</v>
+      </c>
+      <c r="G84" t="s">
+        <v>55</v>
+      </c>
+      <c r="H84" s="2">
         <v>42805</v>
       </c>
-      <c r="I81" s="4">
+      <c r="I84" s="4">
         <v>9.99</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J84" t="s">
         <v>208</v>
       </c>
-      <c r="K81" t="s">
+      <c r="K84" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K81">
-    <sortCondition ref="A2:A81"/>
-    <sortCondition ref="B2:B81"/>
+  <sortState ref="A2:K84">
+    <sortCondition ref="A2:A84"/>
+    <sortCondition ref="B2:B84"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4031,10 +4234,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4098,7 +4301,7 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>74143</v>
       </c>
       <c r="C4" t="s">
@@ -4192,50 +4395,33 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D10" t="s">
         <v>261</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>262</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>269</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="E11" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" t="s">
-        <v>272</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>270</v>
-      </c>
-      <c r="E12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4253,12 +4439,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="10.83203125" style="6"/>
     <col min="2" max="2" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>185</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4266,7 +4452,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>20</v>
       </c>
       <c r="B2" t="s">
@@ -4274,7 +4460,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>48</v>
       </c>
       <c r="B3" t="s">
@@ -4282,7 +4468,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B4" t="s">
@@ -4290,7 +4476,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>15</v>
       </c>
       <c r="B5" t="s">
@@ -4298,7 +4484,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B6" t="s">
@@ -4306,7 +4492,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B7" t="s">
@@ -4314,7 +4500,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>1</v>
       </c>
       <c r="B8" t="s">
@@ -4322,7 +4508,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>1</v>
       </c>
       <c r="B9" t="s">
@@ -4330,7 +4516,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
       <c r="B10" t="s">
@@ -4338,7 +4524,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>3</v>
       </c>
       <c r="B11" t="s">
@@ -4346,7 +4532,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
       <c r="B12" t="s">
@@ -4354,7 +4540,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>2</v>
       </c>
       <c r="B13" t="s">

</xml_diff>

<commit_message>
D&M 5141,  DT&I 12769
</commit_message>
<xml_diff>
--- a/trains/Inventory.xlsx
+++ b/trains/Inventory.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26230"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennismccarthy/WebstormProjects/drm227.github.io/trains/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennismccarthy/All/github/drm227.github.io/trains/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0598AA5-03E4-F744-B641-3307650C2A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locomotives" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Wish List" sheetId="4" r:id="rId3"/>
     <sheet name="EZ Track" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="287">
   <si>
     <t>Road Name</t>
   </si>
@@ -864,12 +865,36 @@
   </si>
   <si>
     <t>eBay - mrisfun</t>
+  </si>
+  <si>
+    <t>heavyweight single window coach</t>
+  </si>
+  <si>
+    <t>dBay</t>
+  </si>
+  <si>
+    <t>$6.24 shipping</t>
+  </si>
+  <si>
+    <t>50' plug door boxcar Stroh's</t>
+  </si>
+  <si>
+    <t>eBay - mowingman35</t>
+  </si>
+  <si>
+    <t>$7 shipping + $2.01 tax</t>
+  </si>
+  <si>
+    <t>100 ton 3-bay hopper</t>
+  </si>
+  <si>
+    <t>gift from Brian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
@@ -961,6 +986,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1287,7 +1315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -1596,7 +1624,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J10">
     <sortCondition ref="A2:A10"/>
     <sortCondition ref="B2:B10"/>
   </sortState>
@@ -1605,12 +1633,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2906,63 +2934,60 @@
         <v>51</v>
       </c>
       <c r="B44">
-        <v>6128</v>
+        <v>5141</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>285</v>
       </c>
       <c r="D44" t="s">
         <v>29</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>139</v>
       </c>
       <c r="F44">
-        <v>97340</v>
+        <v>41714</v>
       </c>
       <c r="G44" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="H44" s="2">
+        <v>44044</v>
       </c>
       <c r="I44" s="4">
-        <v>31.95</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>68</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B45">
-        <v>133</v>
+        <v>6128</v>
       </c>
       <c r="C45" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E45" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="F45">
-        <v>76832</v>
+        <v>97340</v>
       </c>
       <c r="G45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H45" s="2">
-        <v>42770</v>
+        <v>87</v>
       </c>
       <c r="I45" s="4">
-        <v>26.98</v>
+        <v>31.95</v>
       </c>
       <c r="J45" t="s">
-        <v>14</v>
-      </c>
-      <c r="K45" t="s">
-        <v>201</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2970,22 +2995,34 @@
         <v>73</v>
       </c>
       <c r="B46">
-        <v>1165</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>200</v>
       </c>
       <c r="D46" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E46" t="s">
-        <v>76</v>
-      </c>
-      <c r="F46" t="s">
-        <v>77</v>
+        <v>171</v>
+      </c>
+      <c r="F46">
+        <v>76832</v>
       </c>
       <c r="G46" t="s">
-        <v>78</v>
+        <v>55</v>
+      </c>
+      <c r="H46" s="2">
+        <v>42770</v>
+      </c>
+      <c r="I46" s="4">
+        <v>26.98</v>
+      </c>
+      <c r="J46" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2993,31 +3030,22 @@
         <v>73</v>
       </c>
       <c r="B47">
-        <v>9602</v>
+        <v>1165</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47">
-        <v>91487</v>
+        <v>76</v>
+      </c>
+      <c r="F47" t="s">
+        <v>77</v>
       </c>
       <c r="G47" t="s">
-        <v>48</v>
-      </c>
-      <c r="H47" s="2">
-        <v>42309</v>
-      </c>
-      <c r="I47" s="4">
-        <v>16</v>
-      </c>
-      <c r="J47" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -3025,34 +3053,31 @@
         <v>73</v>
       </c>
       <c r="B48">
-        <v>9621</v>
+        <v>9602</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
         <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
-      </c>
-      <c r="F48" t="s">
-        <v>85</v>
+        <v>12</v>
+      </c>
+      <c r="F48">
+        <v>91487</v>
       </c>
       <c r="G48" t="s">
         <v>48</v>
       </c>
       <c r="H48" s="2">
-        <v>42303</v>
+        <v>42309</v>
       </c>
       <c r="I48" s="4">
-        <v>29.95</v>
+        <v>16</v>
       </c>
       <c r="J48" t="s">
-        <v>92</v>
-      </c>
-      <c r="K48" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -3060,28 +3085,34 @@
         <v>73</v>
       </c>
       <c r="B49">
-        <v>10112</v>
+        <v>9621</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49">
-        <v>89082</v>
+        <v>80</v>
+      </c>
+      <c r="F49" t="s">
+        <v>85</v>
       </c>
       <c r="G49" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+      <c r="H49" s="2">
+        <v>42303</v>
       </c>
       <c r="I49" s="4">
-        <v>27.98</v>
+        <v>29.95</v>
       </c>
       <c r="J49" t="s">
-        <v>68</v>
+        <v>92</v>
+      </c>
+      <c r="K49" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -3089,34 +3120,28 @@
         <v>73</v>
       </c>
       <c r="B50">
-        <v>10312</v>
+        <v>10112</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D50" t="s">
         <v>29</v>
       </c>
       <c r="E50" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F50">
-        <v>17532</v>
+        <v>89082</v>
       </c>
       <c r="G50" t="s">
-        <v>87</v>
-      </c>
-      <c r="H50" s="2">
-        <v>42537</v>
+        <v>82</v>
       </c>
       <c r="I50" s="4">
-        <v>11</v>
+        <v>27.98</v>
       </c>
       <c r="J50" t="s">
-        <v>88</v>
-      </c>
-      <c r="K50" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -3124,34 +3149,34 @@
         <v>73</v>
       </c>
       <c r="B51">
-        <v>18055</v>
+        <v>10312</v>
       </c>
       <c r="C51" t="s">
-        <v>248</v>
+        <v>59</v>
       </c>
       <c r="D51" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51">
+        <v>17532</v>
+      </c>
+      <c r="G51" t="s">
+        <v>87</v>
+      </c>
+      <c r="H51" s="2">
+        <v>42537</v>
+      </c>
+      <c r="I51" s="4">
         <v>11</v>
       </c>
-      <c r="E51" t="s">
-        <v>207</v>
-      </c>
-      <c r="F51">
-        <v>6361</v>
-      </c>
-      <c r="G51" t="s">
-        <v>82</v>
-      </c>
-      <c r="H51" s="2">
-        <v>43023</v>
-      </c>
-      <c r="I51" s="4">
-        <v>30</v>
-      </c>
       <c r="J51" t="s">
-        <v>249</v>
+        <v>88</v>
       </c>
       <c r="K51" t="s">
-        <v>250</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -3159,22 +3184,34 @@
         <v>73</v>
       </c>
       <c r="B52">
-        <v>25907</v>
+        <v>12769</v>
       </c>
       <c r="C52" t="s">
-        <v>79</v>
+        <v>282</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>80</v>
-      </c>
-      <c r="F52" t="s">
-        <v>81</v>
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>1076</v>
       </c>
       <c r="G52" t="s">
-        <v>82</v>
+        <v>111</v>
+      </c>
+      <c r="H52" s="2">
+        <v>43892</v>
+      </c>
+      <c r="I52" s="4">
+        <v>32.130000000000003</v>
+      </c>
+      <c r="J52" t="s">
+        <v>283</v>
+      </c>
+      <c r="K52" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -3182,133 +3219,124 @@
         <v>73</v>
       </c>
       <c r="B53">
-        <v>32246</v>
+        <v>18055</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>248</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>24</v>
+        <v>207</v>
       </c>
       <c r="F53">
-        <v>18132</v>
+        <v>6361</v>
       </c>
       <c r="G53" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="2">
+        <v>43023</v>
+      </c>
+      <c r="I53" s="4">
         <v>30</v>
       </c>
-      <c r="H53" s="2">
-        <v>42411</v>
-      </c>
-      <c r="I53" s="4">
-        <v>12.5</v>
-      </c>
       <c r="J53" t="s">
-        <v>90</v>
+        <v>249</v>
       </c>
       <c r="K53" t="s">
-        <v>91</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="B54">
-        <v>5546</v>
+        <v>25907</v>
       </c>
       <c r="C54" t="s">
-        <v>182</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F54" t="s">
-        <v>183</v>
+        <v>81</v>
       </c>
       <c r="G54" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54" s="2">
-        <v>42708</v>
-      </c>
-      <c r="I54" s="4">
-        <v>18</v>
-      </c>
-      <c r="J54" t="s">
-        <v>184</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B55">
-        <v>153</v>
+        <v>32246</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D55" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="F55">
-        <v>11355</v>
+        <v>18132</v>
       </c>
       <c r="G55" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="H55" s="2">
-        <v>43150</v>
+        <v>42411</v>
       </c>
       <c r="I55" s="4">
-        <v>15.27</v>
+        <v>12.5</v>
       </c>
       <c r="J55" t="s">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="K55" t="s">
-        <v>271</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="B56">
-        <v>112115</v>
+        <v>5546</v>
       </c>
       <c r="C56" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="D56" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E56" t="s">
         <v>64</v>
       </c>
       <c r="F56" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="G56" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H56" s="2">
-        <v>46500</v>
+        <v>42708</v>
       </c>
       <c r="I56" s="4">
-        <v>13.6</v>
+        <v>18</v>
       </c>
       <c r="J56" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -3316,34 +3344,34 @@
         <v>22</v>
       </c>
       <c r="B57">
-        <v>112143</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s">
-        <v>231</v>
+        <v>62</v>
       </c>
       <c r="D57" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E57" t="s">
         <v>64</v>
       </c>
-      <c r="F57" t="s">
-        <v>236</v>
+      <c r="F57">
+        <v>11355</v>
       </c>
       <c r="G57" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H57" s="2">
-        <v>42793</v>
+        <v>43150</v>
       </c>
       <c r="I57" s="4">
-        <v>18</v>
+        <v>15.27</v>
       </c>
       <c r="J57" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="K57" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -3351,34 +3379,31 @@
         <v>22</v>
       </c>
       <c r="B58">
-        <v>113894</v>
+        <v>112115</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>231</v>
       </c>
       <c r="D58" t="s">
         <v>29</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58">
-        <v>93725</v>
+        <v>64</v>
+      </c>
+      <c r="F58" t="s">
+        <v>232</v>
       </c>
       <c r="G58" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H58" s="2">
-        <v>42709</v>
+        <v>46500</v>
       </c>
       <c r="I58" s="4">
-        <v>10</v>
+        <v>13.6</v>
       </c>
       <c r="J58" t="s">
-        <v>32</v>
-      </c>
-      <c r="K58" t="s">
-        <v>31</v>
+        <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -3386,25 +3411,34 @@
         <v>22</v>
       </c>
       <c r="B59">
-        <v>148077</v>
+        <v>112143</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="D59" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E59" t="s">
-        <v>44</v>
+        <v>64</v>
+      </c>
+      <c r="F59" t="s">
+        <v>236</v>
       </c>
       <c r="G59" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="H59" s="2">
+        <v>42793</v>
       </c>
       <c r="I59" s="4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J59" t="s">
-        <v>45</v>
+        <v>234</v>
+      </c>
+      <c r="K59" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -3412,34 +3446,34 @@
         <v>22</v>
       </c>
       <c r="B60">
-        <v>302157</v>
+        <v>113894</v>
       </c>
       <c r="C60" t="s">
-        <v>252</v>
+        <v>28</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
       </c>
       <c r="F60">
-        <v>91356</v>
+        <v>93725</v>
       </c>
       <c r="G60" t="s">
         <v>30</v>
       </c>
       <c r="H60" s="2">
-        <v>43029</v>
+        <v>42709</v>
       </c>
       <c r="I60" s="4">
         <v>10</v>
       </c>
       <c r="J60" t="s">
-        <v>253</v>
+        <v>32</v>
       </c>
       <c r="K60" t="s">
-        <v>250</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -3447,34 +3481,25 @@
         <v>22</v>
       </c>
       <c r="B61">
-        <v>591263</v>
+        <v>148077</v>
       </c>
       <c r="C61" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
-      </c>
-      <c r="F61" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G61" t="s">
-        <v>13</v>
-      </c>
-      <c r="H61" s="2">
-        <v>42440</v>
+        <v>30</v>
       </c>
       <c r="I61" s="4">
-        <v>14.99</v>
+        <v>12</v>
       </c>
       <c r="J61" t="s">
-        <v>36</v>
-      </c>
-      <c r="K61" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3482,10 +3507,10 @@
         <v>22</v>
       </c>
       <c r="B62">
-        <v>598016</v>
+        <v>302157</v>
       </c>
       <c r="C62" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -3494,19 +3519,22 @@
         <v>12</v>
       </c>
       <c r="F62">
-        <v>92957</v>
+        <v>91356</v>
       </c>
       <c r="G62" t="s">
         <v>30</v>
       </c>
       <c r="H62" s="2">
-        <v>42680</v>
+        <v>43029</v>
       </c>
       <c r="I62" s="4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J62" t="s">
-        <v>58</v>
+        <v>253</v>
+      </c>
+      <c r="K62" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -3514,45 +3542,45 @@
         <v>22</v>
       </c>
       <c r="B63">
-        <v>675097</v>
+        <v>591263</v>
       </c>
       <c r="C63" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D63" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E63" t="s">
         <v>34</v>
       </c>
       <c r="F63" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G63" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H63" s="2">
-        <v>42521</v>
+        <v>42440</v>
       </c>
       <c r="I63" s="4">
-        <v>16.489999999999998</v>
+        <v>14.99</v>
       </c>
       <c r="J63" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K63" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B64">
-        <v>2706</v>
+        <v>598016</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>230</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -3561,124 +3589,121 @@
         <v>12</v>
       </c>
       <c r="F64">
-        <v>92912</v>
+        <v>92957</v>
       </c>
       <c r="G64" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H64" s="2">
-        <v>42637</v>
+        <v>42680</v>
       </c>
       <c r="I64" s="4">
-        <v>13.29</v>
+        <v>14</v>
       </c>
       <c r="J64" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>242</v>
+        <v>22</v>
       </c>
       <c r="B65">
-        <v>80948</v>
+        <v>675097</v>
       </c>
       <c r="C65" t="s">
-        <v>276</v>
+        <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E65" t="s">
-        <v>12</v>
-      </c>
-      <c r="F65">
-        <v>73518</v>
+        <v>34</v>
+      </c>
+      <c r="F65" t="s">
+        <v>39</v>
       </c>
       <c r="G65" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="H65" s="2">
-        <v>43248</v>
+        <v>42521</v>
       </c>
       <c r="I65" s="4">
-        <v>19.59</v>
+        <v>16.489999999999998</v>
       </c>
       <c r="J65" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="K65" t="s">
-        <v>277</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B66">
-        <v>14274</v>
+        <v>2706</v>
       </c>
       <c r="C66" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D66" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E66" t="s">
         <v>12</v>
       </c>
       <c r="F66">
-        <v>5648</v>
+        <v>92912</v>
       </c>
       <c r="G66" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="H66" s="2">
-        <v>42672</v>
+        <v>42637</v>
       </c>
       <c r="I66" s="4">
-        <v>7</v>
+        <v>13.29</v>
       </c>
       <c r="J66" t="s">
-        <v>49</v>
-      </c>
-      <c r="K66" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
       <c r="B67">
-        <v>14450</v>
+        <v>80948</v>
       </c>
       <c r="C67" t="s">
-        <v>50</v>
+        <v>276</v>
       </c>
       <c r="D67" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E67" t="s">
         <v>12</v>
       </c>
       <c r="F67">
-        <v>5648</v>
+        <v>73518</v>
       </c>
       <c r="G67" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H67" s="2">
-        <v>42672</v>
+        <v>43248</v>
       </c>
       <c r="I67" s="4">
-        <v>7</v>
+        <v>19.59</v>
       </c>
       <c r="J67" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="K67" t="s">
-        <v>66</v>
+        <v>277</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -3686,25 +3711,34 @@
         <v>47</v>
       </c>
       <c r="B68">
-        <v>16534</v>
+        <v>1105</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>279</v>
       </c>
       <c r="D68" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="E68" t="s">
-        <v>53</v>
-      </c>
-      <c r="F68" t="s">
-        <v>157</v>
+        <v>64</v>
+      </c>
+      <c r="F68">
+        <v>20004884</v>
       </c>
       <c r="G68" t="s">
-        <v>48</v>
+        <v>82</v>
+      </c>
+      <c r="H68" s="2">
+        <v>43806</v>
+      </c>
+      <c r="I68" s="4">
+        <v>53.87</v>
       </c>
       <c r="J68" t="s">
-        <v>158</v>
+        <v>280</v>
+      </c>
+      <c r="K68" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -3712,31 +3746,34 @@
         <v>47</v>
       </c>
       <c r="B69">
-        <v>18878</v>
+        <v>1108</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>279</v>
       </c>
       <c r="D69" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E69" t="s">
-        <v>97</v>
-      </c>
-      <c r="F69" t="s">
-        <v>165</v>
+        <v>64</v>
+      </c>
+      <c r="F69">
+        <v>20004885</v>
       </c>
       <c r="G69" t="s">
-        <v>48</v>
+        <v>82</v>
+      </c>
+      <c r="H69" s="2">
+        <v>43806</v>
       </c>
       <c r="I69" s="4">
-        <v>10</v>
+        <v>53.87</v>
       </c>
       <c r="J69" t="s">
-        <v>45</v>
+        <v>280</v>
       </c>
       <c r="K69" t="s">
-        <v>66</v>
+        <v>281</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -3744,28 +3781,31 @@
         <v>47</v>
       </c>
       <c r="B70">
-        <v>18881</v>
+        <v>14274</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>50</v>
       </c>
       <c r="D70" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E70" t="s">
-        <v>97</v>
-      </c>
-      <c r="F70" t="s">
-        <v>166</v>
+        <v>12</v>
+      </c>
+      <c r="F70">
+        <v>5648</v>
       </c>
       <c r="G70" t="s">
         <v>48</v>
       </c>
+      <c r="H70" s="2">
+        <v>42672</v>
+      </c>
       <c r="I70" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J70" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K70" t="s">
         <v>66</v>
@@ -3776,28 +3816,31 @@
         <v>47</v>
       </c>
       <c r="B71">
-        <v>18914</v>
+        <v>14450</v>
       </c>
       <c r="C71" t="s">
-        <v>151</v>
+        <v>50</v>
       </c>
       <c r="D71" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E71" t="s">
-        <v>97</v>
-      </c>
-      <c r="F71" t="s">
-        <v>167</v>
+        <v>12</v>
+      </c>
+      <c r="F71">
+        <v>5648</v>
       </c>
       <c r="G71" t="s">
         <v>48</v>
       </c>
+      <c r="H71" s="2">
+        <v>42672</v>
+      </c>
       <c r="I71" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J71" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K71" t="s">
         <v>66</v>
@@ -3808,31 +3851,25 @@
         <v>47</v>
       </c>
       <c r="B72">
-        <v>18942</v>
+        <v>16534</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="D72" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="E72" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="G72" t="s">
         <v>48</v>
       </c>
-      <c r="I72" s="4">
-        <v>10</v>
-      </c>
       <c r="J72" t="s">
-        <v>45</v>
-      </c>
-      <c r="K72" t="s">
-        <v>66</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -3840,34 +3877,31 @@
         <v>47</v>
       </c>
       <c r="B73">
-        <v>20025</v>
+        <v>18878</v>
       </c>
       <c r="C73" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D73" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E73" t="s">
-        <v>139</v>
-      </c>
-      <c r="F73">
-        <v>41329</v>
+        <v>97</v>
+      </c>
+      <c r="F73" t="s">
+        <v>165</v>
       </c>
       <c r="G73" t="s">
         <v>48</v>
       </c>
-      <c r="H73" s="2">
-        <v>42608</v>
-      </c>
       <c r="I73" s="4">
-        <v>17.989999999999998</v>
+        <v>10</v>
       </c>
       <c r="J73" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="K73" t="s">
-        <v>150</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -3875,34 +3909,31 @@
         <v>47</v>
       </c>
       <c r="B74">
-        <v>20037</v>
+        <v>18881</v>
       </c>
       <c r="C74" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D74" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E74" t="s">
-        <v>139</v>
-      </c>
-      <c r="F74">
-        <v>41330</v>
+        <v>97</v>
+      </c>
+      <c r="F74" t="s">
+        <v>166</v>
       </c>
       <c r="G74" t="s">
         <v>48</v>
       </c>
-      <c r="H74" s="2">
-        <v>42608</v>
-      </c>
       <c r="I74" s="4">
-        <v>17.989999999999998</v>
+        <v>10</v>
       </c>
       <c r="J74" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="K74" t="s">
-        <v>150</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -3910,34 +3941,31 @@
         <v>47</v>
       </c>
       <c r="B75">
-        <v>20045</v>
+        <v>18914</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D75" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E75" t="s">
-        <v>139</v>
-      </c>
-      <c r="F75">
-        <v>41331</v>
+        <v>97</v>
+      </c>
+      <c r="F75" t="s">
+        <v>167</v>
       </c>
       <c r="G75" t="s">
         <v>48</v>
       </c>
-      <c r="H75" s="2">
-        <v>42608</v>
-      </c>
       <c r="I75" s="4">
-        <v>17.989999999999998</v>
+        <v>10</v>
       </c>
       <c r="J75" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="K75" t="s">
-        <v>150</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -3945,34 +3973,31 @@
         <v>47</v>
       </c>
       <c r="B76">
-        <v>30196</v>
+        <v>18942</v>
       </c>
       <c r="C76" t="s">
-        <v>202</v>
+        <v>151</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E76" t="s">
-        <v>171</v>
-      </c>
-      <c r="F76">
-        <v>84189</v>
+        <v>97</v>
+      </c>
+      <c r="F76" t="s">
+        <v>168</v>
       </c>
       <c r="G76" t="s">
-        <v>55</v>
-      </c>
-      <c r="H76" s="2">
-        <v>43232</v>
+        <v>48</v>
       </c>
       <c r="I76" s="4">
-        <v>34.56</v>
+        <v>10</v>
       </c>
       <c r="J76" t="s">
-        <v>278</v>
+        <v>45</v>
       </c>
       <c r="K76" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3980,28 +4005,34 @@
         <v>47</v>
       </c>
       <c r="B77">
-        <v>83873</v>
+        <v>20025</v>
       </c>
       <c r="C77" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D77" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E77" t="s">
-        <v>53</v>
-      </c>
-      <c r="F77" t="s">
-        <v>154</v>
+        <v>139</v>
+      </c>
+      <c r="F77">
+        <v>41329</v>
       </c>
       <c r="G77" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H77" s="2">
+        <v>42608</v>
       </c>
       <c r="I77" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J77" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K77" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -4009,28 +4040,34 @@
         <v>47</v>
       </c>
       <c r="B78">
-        <v>83916</v>
+        <v>20037</v>
       </c>
       <c r="C78" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D78" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E78" t="s">
-        <v>53</v>
-      </c>
-      <c r="F78" t="s">
-        <v>155</v>
+        <v>139</v>
+      </c>
+      <c r="F78">
+        <v>41330</v>
       </c>
       <c r="G78" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H78" s="2">
+        <v>42608</v>
       </c>
       <c r="I78" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J78" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K78" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -4038,28 +4075,34 @@
         <v>47</v>
       </c>
       <c r="B79">
-        <v>83950</v>
+        <v>20045</v>
       </c>
       <c r="C79" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E79" t="s">
-        <v>53</v>
-      </c>
-      <c r="F79" t="s">
-        <v>152</v>
+        <v>139</v>
+      </c>
+      <c r="F79">
+        <v>41331</v>
       </c>
       <c r="G79" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="H79" s="2">
+        <v>42608</v>
       </c>
       <c r="I79" s="4">
-        <v>23.95</v>
+        <v>17.989999999999998</v>
       </c>
       <c r="J79" t="s">
-        <v>68</v>
+        <v>149</v>
+      </c>
+      <c r="K79" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -4067,165 +4110,287 @@
         <v>47</v>
       </c>
       <c r="B80">
-        <v>83987</v>
+        <v>30196</v>
       </c>
       <c r="C80" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="D80" t="s">
         <v>11</v>
       </c>
       <c r="E80" t="s">
-        <v>53</v>
-      </c>
-      <c r="F80" t="s">
-        <v>153</v>
+        <v>171</v>
+      </c>
+      <c r="F80">
+        <v>84189</v>
       </c>
       <c r="G80" t="s">
         <v>55</v>
       </c>
+      <c r="H80" s="2">
+        <v>43232</v>
+      </c>
       <c r="I80" s="4">
-        <v>23.95</v>
+        <v>34.56</v>
       </c>
       <c r="J80" t="s">
-        <v>68</v>
+        <v>278</v>
+      </c>
+      <c r="K80" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>47</v>
       </c>
-      <c r="B81" t="s">
-        <v>161</v>
+      <c r="B81">
+        <v>83873</v>
       </c>
       <c r="C81" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D81" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E81" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="F81" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G81" t="s">
         <v>55</v>
       </c>
+      <c r="I81" s="4">
+        <v>23.95</v>
+      </c>
       <c r="J81" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>47</v>
       </c>
-      <c r="B82" t="s">
-        <v>159</v>
+      <c r="B82">
+        <v>83916</v>
       </c>
       <c r="C82" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="D82" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="E82" t="s">
-        <v>64</v>
-      </c>
-      <c r="F82">
-        <v>11347</v>
+        <v>53</v>
+      </c>
+      <c r="F82" t="s">
+        <v>155</v>
       </c>
       <c r="G82" t="s">
         <v>55</v>
       </c>
-      <c r="H82" s="2">
-        <v>42170</v>
-      </c>
       <c r="I82" s="4">
-        <v>21.5</v>
+        <v>23.95</v>
       </c>
       <c r="J82" t="s">
-        <v>160</v>
-      </c>
-      <c r="K82" t="s">
-        <v>164</v>
+        <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>239</v>
+        <v>47</v>
       </c>
       <c r="B83">
-        <v>70055</v>
+        <v>83950</v>
       </c>
       <c r="C83" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D83" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E83" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F83" t="s">
-        <v>240</v>
+        <v>152</v>
       </c>
       <c r="G83" t="s">
-        <v>19</v>
-      </c>
-      <c r="H83" s="2">
-        <v>42868</v>
+        <v>55</v>
       </c>
       <c r="I83" s="4">
-        <v>15.41</v>
+        <v>23.95</v>
       </c>
       <c r="J83" t="s">
-        <v>14</v>
-      </c>
-      <c r="K83" t="s">
-        <v>241</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>206</v>
+        <v>47</v>
       </c>
       <c r="B84">
-        <v>41912</v>
+        <v>83987</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
       </c>
       <c r="E84" t="s">
-        <v>207</v>
-      </c>
-      <c r="F84">
-        <v>40931302</v>
+        <v>53</v>
+      </c>
+      <c r="F84" t="s">
+        <v>153</v>
       </c>
       <c r="G84" t="s">
         <v>55</v>
       </c>
-      <c r="H84" s="2">
+      <c r="I84" s="4">
+        <v>23.95</v>
+      </c>
+      <c r="J84" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>47</v>
+      </c>
+      <c r="B85" t="s">
+        <v>161</v>
+      </c>
+      <c r="C85" t="s">
+        <v>162</v>
+      </c>
+      <c r="D85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" t="s">
+        <v>76</v>
+      </c>
+      <c r="F85" t="s">
+        <v>163</v>
+      </c>
+      <c r="G85" t="s">
+        <v>55</v>
+      </c>
+      <c r="J85" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>47</v>
+      </c>
+      <c r="B86" t="s">
+        <v>159</v>
+      </c>
+      <c r="C86" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" t="s">
+        <v>64</v>
+      </c>
+      <c r="F86">
+        <v>11347</v>
+      </c>
+      <c r="G86" t="s">
+        <v>55</v>
+      </c>
+      <c r="H86" s="2">
+        <v>42170</v>
+      </c>
+      <c r="I86" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="J86" t="s">
+        <v>160</v>
+      </c>
+      <c r="K86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>239</v>
+      </c>
+      <c r="B87">
+        <v>70055</v>
+      </c>
+      <c r="C87" t="s">
+        <v>134</v>
+      </c>
+      <c r="D87" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" t="s">
+        <v>34</v>
+      </c>
+      <c r="F87" t="s">
+        <v>240</v>
+      </c>
+      <c r="G87" t="s">
+        <v>19</v>
+      </c>
+      <c r="H87" s="2">
+        <v>42868</v>
+      </c>
+      <c r="I87" s="4">
+        <v>15.41</v>
+      </c>
+      <c r="J87" t="s">
+        <v>14</v>
+      </c>
+      <c r="K87" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>206</v>
+      </c>
+      <c r="B88">
+        <v>41912</v>
+      </c>
+      <c r="C88" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" t="s">
+        <v>207</v>
+      </c>
+      <c r="F88">
+        <v>40931302</v>
+      </c>
+      <c r="G88" t="s">
+        <v>55</v>
+      </c>
+      <c r="H88" s="2">
         <v>42805</v>
       </c>
-      <c r="I84" s="4">
+      <c r="I88" s="4">
         <v>9.99</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J88" t="s">
         <v>208</v>
       </c>
-      <c r="K84" t="s">
+      <c r="K88" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K84">
-    <sortCondition ref="A2:A84"/>
-    <sortCondition ref="B2:B84"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K88">
+    <sortCondition ref="A2:A88"/>
+    <sortCondition ref="B2:B88"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4233,7 +4398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -4430,7 +4595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
added Michigan Alkali tank car
</commit_message>
<xml_diff>
--- a/trains/Inventory.xlsx
+++ b/trains/Inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennismccarthy/All/github/drm227.github.io/trains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0598AA5-03E4-F744-B641-3307650C2A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34E65DB-F519-D14C-9E8E-1141FB60117E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="291">
   <si>
     <t>Road Name</t>
   </si>
@@ -889,6 +889,18 @@
   </si>
   <si>
     <t>gift from Brian</t>
+  </si>
+  <si>
+    <t>GATX</t>
+  </si>
+  <si>
+    <t>train show - Colorado Springs</t>
+  </si>
+  <si>
+    <t>Athearn or AHM?</t>
+  </si>
+  <si>
+    <t>1551 or 5276 ?</t>
   </si>
 </sst>
 </file>
@@ -1634,11 +1646,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4385,6 +4397,35 @@
       </c>
       <c r="K88" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>287</v>
+      </c>
+      <c r="B89">
+        <v>32313</v>
+      </c>
+      <c r="D89" t="s">
+        <v>96</v>
+      </c>
+      <c r="E89" t="s">
+        <v>289</v>
+      </c>
+      <c r="F89" t="s">
+        <v>290</v>
+      </c>
+      <c r="G89" t="s">
+        <v>111</v>
+      </c>
+      <c r="H89" s="2">
+        <v>44591</v>
+      </c>
+      <c r="I89" s="4">
+        <v>12</v>
+      </c>
+      <c r="J89" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>